<commit_message>
loaded data set and rounded up values
</commit_message>
<xml_diff>
--- a/budgetusd.xlsx
+++ b/budgetusd.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielporras/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDF50476-08F9-0B45-BA04-CEDD75E9B000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC47857C-1C7B-3249-8049-CB5DA96C4B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14840" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
+    <workbookView xWindow="4640" yWindow="500" windowWidth="18620" windowHeight="13140" activeTab="1" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="Revenue" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -174,19 +175,129 @@
   </si>
   <si>
     <t>2022-12</t>
+  </si>
+  <si>
+    <t>Percentage %</t>
+  </si>
+  <si>
+    <t>Winter North</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Holidays North</t>
+  </si>
+  <si>
+    <t>Holidays Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Local Rainy Season</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>International Flights</t>
+  </si>
+  <si>
+    <t>2023-01</t>
+  </si>
+  <si>
+    <t>2023-02</t>
+  </si>
+  <si>
+    <t>2023-03</t>
+  </si>
+  <si>
+    <t>2023-04</t>
+  </si>
+  <si>
+    <t>2023-05</t>
+  </si>
+  <si>
+    <t>2023-06</t>
+  </si>
+  <si>
+    <t>2023-07</t>
+  </si>
+  <si>
+    <t>2023-08</t>
+  </si>
+  <si>
+    <t>2023-09</t>
+  </si>
+  <si>
+    <t>2023-10</t>
+  </si>
+  <si>
+    <t>2023-11</t>
+  </si>
+  <si>
+    <t>2023-12</t>
+  </si>
+  <si>
+    <t>Marketing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="mmm/yyyy"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,9 +320,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,13 +647,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17AB7571-518D-374C-8FD9-00C835832375}">
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI19" sqref="AI19"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="21" max="21" width="31.6640625" customWidth="1"/>
+    <col min="25" max="25" width="18" customWidth="1"/>
+    <col min="26" max="26" width="18.1640625" customWidth="1"/>
+    <col min="27" max="27" width="19.1640625" customWidth="1"/>
+    <col min="28" max="28" width="21" customWidth="1"/>
+    <col min="29" max="30" width="15.6640625" customWidth="1"/>
+    <col min="31" max="31" width="17.33203125" customWidth="1"/>
+    <col min="32" max="32" width="16" customWidth="1"/>
+    <col min="33" max="33" width="14.5" customWidth="1"/>
+    <col min="34" max="34" width="16.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -639,8 +782,8 @@
       </c>
     </row>
     <row r="2" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
+      <c r="A2" s="7">
+        <v>44562</v>
       </c>
       <c r="B2" s="1">
         <v>7771.6388888888887</v>
@@ -743,8 +886,8 @@
       </c>
     </row>
     <row r="3" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
+      <c r="A3" s="7">
+        <v>44593</v>
       </c>
       <c r="B3" s="1">
         <v>5660</v>
@@ -847,8 +990,8 @@
       </c>
     </row>
     <row r="4" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>36</v>
+      <c r="A4" s="7">
+        <v>44621</v>
       </c>
       <c r="B4" s="1">
         <v>5299.8611111111113</v>
@@ -951,8 +1094,8 @@
       </c>
     </row>
     <row r="5" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
+      <c r="A5" s="7">
+        <v>44652</v>
       </c>
       <c r="B5" s="1">
         <v>11300.75</v>
@@ -1055,8 +1198,8 @@
       </c>
     </row>
     <row r="6" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>38</v>
+      <c r="A6" s="7">
+        <v>44682</v>
       </c>
       <c r="B6" s="1">
         <v>5555.0099999999993</v>
@@ -1159,8 +1302,8 @@
       </c>
     </row>
     <row r="7" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
+      <c r="A7" s="7">
+        <v>44713</v>
       </c>
       <c r="B7" s="1">
         <v>2821.9919444444445</v>
@@ -1263,8 +1406,8 @@
       </c>
     </row>
     <row r="8" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>40</v>
+      <c r="A8" s="7">
+        <v>44743</v>
       </c>
       <c r="B8" s="1">
         <v>6345.9894444444444</v>
@@ -1367,8 +1510,8 @@
       </c>
     </row>
     <row r="9" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>41</v>
+      <c r="A9" s="7">
+        <v>44774</v>
       </c>
       <c r="B9" s="1">
         <v>5398.0031388888892</v>
@@ -1471,8 +1614,8 @@
       </c>
     </row>
     <row r="10" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>42</v>
+      <c r="A10" s="7">
+        <v>44805</v>
       </c>
       <c r="B10" s="1">
         <v>5495.2106666666668</v>
@@ -1575,8 +1718,8 @@
       </c>
     </row>
     <row r="11" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>43</v>
+      <c r="A11" s="7">
+        <v>44835</v>
       </c>
       <c r="B11" s="1">
         <v>3969.1485638888894</v>
@@ -1679,8 +1822,8 @@
       </c>
     </row>
     <row r="12" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>44</v>
+      <c r="A12" s="7">
+        <v>44866</v>
       </c>
       <c r="B12" s="1">
         <v>5675.9397222222215</v>
@@ -1783,8 +1926,8 @@
       </c>
     </row>
     <row r="13" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>45</v>
+      <c r="A13" s="7">
+        <v>44896</v>
       </c>
       <c r="B13" s="1">
         <v>8197.7705555555549</v>
@@ -1886,7 +2029,1010 @@
         <v>12391.600378027781</v>
       </c>
     </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>45231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>45261</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE46400-3D03-3941-9442-654DF1291CF8}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="5" customWidth="1"/>
+    <col min="4" max="5" width="23.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25" style="5" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="5" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8">
+        <v>62.111111111111114</v>
+      </c>
+      <c r="I2" s="8">
+        <v>7771.6388888888887</v>
+      </c>
+      <c r="J2" s="8">
+        <v>3972.5555555555557</v>
+      </c>
+      <c r="K2" s="8">
+        <v>13136.888888888889</v>
+      </c>
+      <c r="L2" s="8">
+        <v>24881.083333333332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
+        <v>62.111111111111114</v>
+      </c>
+      <c r="I3" s="8">
+        <v>5660</v>
+      </c>
+      <c r="J3" s="8">
+        <v>3773.3333333333335</v>
+      </c>
+      <c r="K3" s="8">
+        <v>11430.527777777777</v>
+      </c>
+      <c r="L3" s="8">
+        <v>20863.861111111109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8">
+        <v>99.305555555555557</v>
+      </c>
+      <c r="I4" s="8">
+        <v>5299.8611111111113</v>
+      </c>
+      <c r="J4" s="8">
+        <v>3533.2222222222222</v>
+      </c>
+      <c r="K4" s="8">
+        <v>9742.6111111111113</v>
+      </c>
+      <c r="L4" s="8">
+        <v>18575.694444444445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8">
+        <v>246.05555555555554</v>
+      </c>
+      <c r="I5" s="8">
+        <v>11300.75</v>
+      </c>
+      <c r="J5" s="8">
+        <v>7533.833333333333</v>
+      </c>
+      <c r="K5" s="8">
+        <v>15043.805555555555</v>
+      </c>
+      <c r="L5" s="8">
+        <v>33878.388888888891</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>144.92038888888888</v>
+      </c>
+      <c r="I6" s="8">
+        <v>5555.0099999999993</v>
+      </c>
+      <c r="J6" s="8">
+        <v>3703.3399999999997</v>
+      </c>
+      <c r="K6" s="8">
+        <v>8546.1691666666666</v>
+      </c>
+      <c r="L6" s="8">
+        <v>17804.519166666665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>118.45822222222222</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2821.9919444444445</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1881.3280555555555</v>
+      </c>
+      <c r="K7" s="8">
+        <v>7171.4191666666666</v>
+      </c>
+      <c r="L7" s="8">
+        <v>11874.739166666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="3">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <v>46.761375416666667</v>
+      </c>
+      <c r="I8" s="8">
+        <v>6345.9894444444444</v>
+      </c>
+      <c r="J8" s="8">
+        <v>4230.6597222222226</v>
+      </c>
+      <c r="K8" s="8">
+        <v>15864.97388888889</v>
+      </c>
+      <c r="L8" s="8">
+        <v>26441.623055555556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="3">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8">
+        <v>149.96791666666667</v>
+      </c>
+      <c r="I9" s="8">
+        <v>5398.0031388888892</v>
+      </c>
+      <c r="J9" s="8">
+        <v>3598.6686111111112</v>
+      </c>
+      <c r="K9" s="8">
+        <v>11925.820833333333</v>
+      </c>
+      <c r="L9" s="8">
+        <v>20922.492583333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>170.24083333333334</v>
+      </c>
+      <c r="I10" s="8">
+        <v>5495.2106666666668</v>
+      </c>
+      <c r="J10" s="8">
+        <v>3663.4737777777782</v>
+      </c>
+      <c r="K10" s="8">
+        <v>13738.026666666667</v>
+      </c>
+      <c r="L10" s="8">
+        <v>22896.711111111115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8">
+        <v>176.07463058333332</v>
+      </c>
+      <c r="I11" s="8">
+        <v>3969.1485638888894</v>
+      </c>
+      <c r="J11" s="8">
+        <v>2646.0990422222221</v>
+      </c>
+      <c r="K11" s="8">
+        <v>7765.7254499999999</v>
+      </c>
+      <c r="L11" s="8">
+        <v>14380.973056111112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="H12" s="8">
+        <v>176.07463058333332</v>
+      </c>
+      <c r="I12" s="8">
+        <v>5675.9397222222215</v>
+      </c>
+      <c r="J12" s="8">
+        <v>3783.9597222222219</v>
+      </c>
+      <c r="K12" s="8">
+        <v>14796.252777777778</v>
+      </c>
+      <c r="L12" s="8">
+        <v>24256.152222222223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="3">
+        <v>10</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+      <c r="H13" s="8">
+        <v>196.63585922222222</v>
+      </c>
+      <c r="I13" s="8">
+        <v>8197.7705555555549</v>
+      </c>
+      <c r="J13" s="8">
+        <v>5465.1805555555557</v>
+      </c>
+      <c r="K13" s="8">
+        <v>16039.116388888888</v>
+      </c>
+      <c r="L13" s="8">
+        <v>29702.067499999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="3">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="3">
+        <v>4</v>
+      </c>
+      <c r="H14" s="8">
+        <v>277.43523555555555</v>
+      </c>
+      <c r="I14" s="8">
+        <v>11362.223050000001</v>
+      </c>
+      <c r="J14" s="8">
+        <v>4926.2308388888887</v>
+      </c>
+      <c r="K14" s="8">
+        <v>18609.989444444444</v>
+      </c>
+      <c r="L14" s="8">
+        <v>34898.443333333329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.82</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="3">
+        <v>4</v>
+      </c>
+      <c r="H15" s="8">
+        <v>583.33333333333337</v>
+      </c>
+      <c r="I15" s="8">
+        <v>6112.6362361111114</v>
+      </c>
+      <c r="J15" s="8">
+        <v>4075.0908250000002</v>
+      </c>
+      <c r="K15" s="8">
+        <v>16622.081111111111</v>
+      </c>
+      <c r="L15" s="8">
+        <v>26809.808172222223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="3">
+        <v>4</v>
+      </c>
+      <c r="H16" s="8">
+        <v>189.90263766666666</v>
+      </c>
+      <c r="I16" s="8">
+        <v>7636.8269341522582</v>
+      </c>
+      <c r="J16" s="8">
+        <v>5603.8833169390737</v>
+      </c>
+      <c r="K16" s="8">
+        <v>21306.423360019777</v>
+      </c>
+      <c r="L16" s="8">
+        <v>34547.133611111116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="C17" s="3">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="3">
+        <v>4</v>
+      </c>
+      <c r="H17" s="8">
+        <v>339.38964222222216</v>
+      </c>
+      <c r="I17" s="8">
+        <v>10182.808819444444</v>
+      </c>
+      <c r="J17" s="8">
+        <v>6788.5391666666665</v>
+      </c>
+      <c r="K17" s="8">
+        <v>17039.369466666667</v>
+      </c>
+      <c r="L17" s="8">
+        <v>34010.717452777775</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="3">
+        <v>4</v>
+      </c>
+      <c r="H18" s="8">
+        <v>366.89441874999994</v>
+      </c>
+      <c r="I18" s="8">
+        <v>7338.333333333333</v>
+      </c>
+      <c r="J18" s="8">
+        <v>5283.6402777777776</v>
+      </c>
+      <c r="K18" s="8">
+        <v>16731.527777777777</v>
+      </c>
+      <c r="L18" s="8">
+        <v>29353.50138888889</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="3">
+        <v>4</v>
+      </c>
+      <c r="H19" s="8">
+        <v>289.95980819444441</v>
+      </c>
+      <c r="I19" s="8">
+        <v>6458.8563888888884</v>
+      </c>
+      <c r="J19" s="8">
+        <v>4085.951111111111</v>
+      </c>
+      <c r="K19" s="8">
+        <v>15332.020833333334</v>
+      </c>
+      <c r="L19" s="8">
+        <v>25876.828333333331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="3">
+        <v>20</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="3">
+        <v>4</v>
+      </c>
+      <c r="H20" s="8">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I20" s="8">
+        <v>7797.3772222222224</v>
+      </c>
+      <c r="J20" s="8">
+        <v>5928.2080555555549</v>
+      </c>
+      <c r="K20" s="8">
+        <v>20746.446944444444</v>
+      </c>
+      <c r="L20" s="8">
+        <v>34472.032222222217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="3">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="3">
+        <v>4</v>
+      </c>
+      <c r="H21" s="8">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I21" s="3">
+        <v>6000</v>
+      </c>
+      <c r="J21" s="3">
+        <v>5000</v>
+      </c>
+      <c r="K21" s="3">
+        <v>17000</v>
+      </c>
+      <c r="L21" s="3">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
+        <v>3</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="3">
+        <v>4</v>
+      </c>
+      <c r="H22" s="8">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="8">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="3">
+        <v>4</v>
+      </c>
+      <c r="H24" s="8">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="3">
+        <v>10</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4</v>
+      </c>
+      <c r="H25" s="8">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
performed exploratory data analysis
</commit_message>
<xml_diff>
--- a/budgetusd.xlsx
+++ b/budgetusd.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielporras/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC47857C-1C7B-3249-8049-CB5DA96C4B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D974A011-0678-6148-8728-4B4A3CB74B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="500" windowWidth="18620" windowHeight="13140" activeTab="1" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="Revenue" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Holidays Local</t>
   </si>
   <si>
-    <t xml:space="preserve"> Local Rainy Season</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -241,6 +238,15 @@
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>Local Rainy Season</t>
+  </si>
+  <si>
+    <t>Average F&amp;B</t>
+  </si>
+  <si>
+    <t>ARR</t>
   </si>
 </sst>
 </file>
@@ -248,9 +254,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="mmm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -299,6 +305,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -317,10 +330,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -328,14 +342,16 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2097,11 +2113,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE46400-3D03-3941-9442-654DF1291CF8}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2112,13 +2126,15 @@
     <col min="6" max="6" width="25" style="5" customWidth="1"/>
     <col min="7" max="7" width="25.1640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2135,28 +2151,34 @@
         <v>50</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
@@ -2182,19 +2204,25 @@
         <v>62.111111111111114</v>
       </c>
       <c r="I2" s="8">
+        <v>15</v>
+      </c>
+      <c r="J2" s="8">
+        <v>75</v>
+      </c>
+      <c r="K2" s="8">
         <v>7771.6388888888887</v>
       </c>
-      <c r="J2" s="8">
+      <c r="L2" s="8">
         <v>3972.5555555555557</v>
       </c>
-      <c r="K2" s="8">
+      <c r="M2" s="8">
         <v>13136.888888888889</v>
       </c>
-      <c r="L2" s="8">
+      <c r="N2" s="8">
         <v>24881.083333333332</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -2220,19 +2248,25 @@
         <v>62.111111111111114</v>
       </c>
       <c r="I3" s="8">
+        <v>15</v>
+      </c>
+      <c r="J3" s="8">
+        <v>75</v>
+      </c>
+      <c r="K3" s="8">
         <v>5660</v>
       </c>
-      <c r="J3" s="8">
+      <c r="L3" s="8">
         <v>3773.3333333333335</v>
       </c>
-      <c r="K3" s="8">
+      <c r="M3" s="8">
         <v>11430.527777777777</v>
       </c>
-      <c r="L3" s="8">
+      <c r="N3" s="8">
         <v>20863.861111111109</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
@@ -2258,19 +2292,25 @@
         <v>99.305555555555557</v>
       </c>
       <c r="I4" s="8">
+        <v>15</v>
+      </c>
+      <c r="J4" s="8">
+        <v>75</v>
+      </c>
+      <c r="K4" s="8">
         <v>5299.8611111111113</v>
       </c>
-      <c r="J4" s="8">
+      <c r="L4" s="8">
         <v>3533.2222222222222</v>
       </c>
-      <c r="K4" s="8">
+      <c r="M4" s="8">
         <v>9742.6111111111113</v>
       </c>
-      <c r="L4" s="8">
+      <c r="N4" s="8">
         <v>18575.694444444445</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>37</v>
       </c>
@@ -2296,19 +2336,25 @@
         <v>246.05555555555554</v>
       </c>
       <c r="I5" s="8">
+        <v>15</v>
+      </c>
+      <c r="J5" s="8">
+        <v>75</v>
+      </c>
+      <c r="K5" s="8">
         <v>11300.75</v>
       </c>
-      <c r="J5" s="8">
+      <c r="L5" s="8">
         <v>7533.833333333333</v>
       </c>
-      <c r="K5" s="8">
+      <c r="M5" s="8">
         <v>15043.805555555555</v>
       </c>
-      <c r="L5" s="8">
+      <c r="N5" s="8">
         <v>33878.388888888891</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>38</v>
       </c>
@@ -2325,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -2334,19 +2380,25 @@
         <v>144.92038888888888</v>
       </c>
       <c r="I6" s="8">
+        <v>15</v>
+      </c>
+      <c r="J6" s="8">
+        <v>75</v>
+      </c>
+      <c r="K6" s="8">
         <v>5555.0099999999993</v>
       </c>
-      <c r="J6" s="8">
+      <c r="L6" s="8">
         <v>3703.3399999999997</v>
       </c>
-      <c r="K6" s="8">
+      <c r="M6" s="8">
         <v>8546.1691666666666</v>
       </c>
-      <c r="L6" s="8">
+      <c r="N6" s="8">
         <v>17804.519166666665</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>39</v>
       </c>
@@ -2363,7 +2415,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -2372,19 +2424,25 @@
         <v>118.45822222222222</v>
       </c>
       <c r="I7" s="8">
+        <v>15</v>
+      </c>
+      <c r="J7" s="8">
+        <v>75</v>
+      </c>
+      <c r="K7" s="8">
         <v>2821.9919444444445</v>
       </c>
-      <c r="J7" s="8">
+      <c r="L7" s="8">
         <v>1881.3280555555555</v>
       </c>
-      <c r="K7" s="8">
+      <c r="M7" s="8">
         <v>7171.4191666666666</v>
       </c>
-      <c r="L7" s="8">
+      <c r="N7" s="8">
         <v>11874.739166666666</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>40</v>
       </c>
@@ -2401,7 +2459,7 @@
         <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -2410,19 +2468,25 @@
         <v>46.761375416666667</v>
       </c>
       <c r="I8" s="8">
+        <v>17</v>
+      </c>
+      <c r="J8" s="8">
+        <v>75</v>
+      </c>
+      <c r="K8" s="8">
         <v>6345.9894444444444</v>
       </c>
-      <c r="J8" s="8">
+      <c r="L8" s="8">
         <v>4230.6597222222226</v>
       </c>
-      <c r="K8" s="8">
+      <c r="M8" s="8">
         <v>15864.97388888889</v>
       </c>
-      <c r="L8" s="8">
+      <c r="N8" s="8">
         <v>26441.623055555556</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
@@ -2439,7 +2503,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -2448,19 +2512,25 @@
         <v>149.96791666666667</v>
       </c>
       <c r="I9" s="8">
+        <v>17</v>
+      </c>
+      <c r="J9" s="8">
+        <v>77</v>
+      </c>
+      <c r="K9" s="8">
         <v>5398.0031388888892</v>
       </c>
-      <c r="J9" s="8">
+      <c r="L9" s="8">
         <v>3598.6686111111112</v>
       </c>
-      <c r="K9" s="8">
+      <c r="M9" s="8">
         <v>11925.820833333333</v>
       </c>
-      <c r="L9" s="8">
+      <c r="N9" s="8">
         <v>20922.492583333333</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>42</v>
       </c>
@@ -2486,19 +2556,25 @@
         <v>170.24083333333334</v>
       </c>
       <c r="I10" s="8">
+        <v>17</v>
+      </c>
+      <c r="J10" s="8">
+        <v>77</v>
+      </c>
+      <c r="K10" s="8">
         <v>5495.2106666666668</v>
       </c>
-      <c r="J10" s="8">
+      <c r="L10" s="8">
         <v>3663.4737777777782</v>
       </c>
-      <c r="K10" s="8">
+      <c r="M10" s="8">
         <v>13738.026666666667</v>
       </c>
-      <c r="L10" s="8">
+      <c r="N10" s="8">
         <v>22896.711111111115</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>43</v>
       </c>
@@ -2524,19 +2600,25 @@
         <v>176.07463058333332</v>
       </c>
       <c r="I11" s="8">
+        <v>17</v>
+      </c>
+      <c r="J11" s="8">
+        <v>77</v>
+      </c>
+      <c r="K11" s="8">
         <v>3969.1485638888894</v>
       </c>
-      <c r="J11" s="8">
+      <c r="L11" s="8">
         <v>2646.0990422222221</v>
       </c>
-      <c r="K11" s="8">
+      <c r="M11" s="8">
         <v>7765.7254499999999</v>
       </c>
-      <c r="L11" s="8">
+      <c r="N11" s="8">
         <v>14380.973056111112</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>44</v>
       </c>
@@ -2562,19 +2644,25 @@
         <v>176.07463058333332</v>
       </c>
       <c r="I12" s="8">
+        <v>17</v>
+      </c>
+      <c r="J12" s="8">
+        <v>77</v>
+      </c>
+      <c r="K12" s="8">
         <v>5675.9397222222215</v>
       </c>
-      <c r="J12" s="8">
+      <c r="L12" s="8">
         <v>3783.9597222222219</v>
       </c>
-      <c r="K12" s="8">
+      <c r="M12" s="8">
         <v>14796.252777777778</v>
       </c>
-      <c r="L12" s="8">
+      <c r="N12" s="8">
         <v>24256.152222222223</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>45</v>
       </c>
@@ -2600,21 +2688,27 @@
         <v>196.63585922222222</v>
       </c>
       <c r="I13" s="8">
+        <v>17</v>
+      </c>
+      <c r="J13" s="8">
+        <v>77</v>
+      </c>
+      <c r="K13" s="8">
         <v>8197.7705555555549</v>
       </c>
-      <c r="J13" s="8">
+      <c r="L13" s="8">
         <v>5465.1805555555557</v>
       </c>
-      <c r="K13" s="8">
+      <c r="M13" s="8">
         <v>16039.116388888888</v>
       </c>
-      <c r="L13" s="8">
+      <c r="N13" s="8">
         <v>29702.067499999997</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4">
         <v>0.81</v>
@@ -2638,21 +2732,27 @@
         <v>277.43523555555555</v>
       </c>
       <c r="I14" s="8">
+        <v>19</v>
+      </c>
+      <c r="J14" s="8">
+        <v>79</v>
+      </c>
+      <c r="K14" s="8">
         <v>11362.223050000001</v>
       </c>
-      <c r="J14" s="8">
+      <c r="L14" s="8">
         <v>4926.2308388888887</v>
       </c>
-      <c r="K14" s="8">
+      <c r="M14" s="8">
         <v>18609.989444444444</v>
       </c>
-      <c r="L14" s="8">
+      <c r="N14" s="8">
         <v>34898.443333333329</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="4">
         <v>0.82</v>
@@ -2676,21 +2776,27 @@
         <v>583.33333333333337</v>
       </c>
       <c r="I15" s="8">
+        <v>19</v>
+      </c>
+      <c r="J15" s="8">
+        <v>79</v>
+      </c>
+      <c r="K15" s="8">
         <v>6112.6362361111114</v>
       </c>
-      <c r="J15" s="8">
+      <c r="L15" s="8">
         <v>4075.0908250000002</v>
       </c>
-      <c r="K15" s="8">
+      <c r="M15" s="8">
         <v>16622.081111111111</v>
       </c>
-      <c r="L15" s="8">
+      <c r="N15" s="8">
         <v>26809.808172222223</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="4">
         <v>0.73</v>
@@ -2714,21 +2820,27 @@
         <v>189.90263766666666</v>
       </c>
       <c r="I16" s="8">
+        <v>19</v>
+      </c>
+      <c r="J16" s="8">
+        <v>79</v>
+      </c>
+      <c r="K16" s="8">
         <v>7636.8269341522582</v>
       </c>
-      <c r="J16" s="8">
+      <c r="L16" s="8">
         <v>5603.8833169390737</v>
       </c>
-      <c r="K16" s="8">
+      <c r="M16" s="8">
         <v>21306.423360019777</v>
       </c>
-      <c r="L16" s="8">
+      <c r="N16" s="8">
         <v>34547.133611111116</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4">
         <v>0.78</v>
@@ -2752,21 +2864,27 @@
         <v>339.38964222222216</v>
       </c>
       <c r="I17" s="8">
+        <v>19</v>
+      </c>
+      <c r="J17" s="8">
+        <v>79</v>
+      </c>
+      <c r="K17" s="8">
         <v>10182.808819444444</v>
       </c>
-      <c r="J17" s="8">
+      <c r="L17" s="8">
         <v>6788.5391666666665</v>
       </c>
-      <c r="K17" s="8">
+      <c r="M17" s="8">
         <v>17039.369466666667</v>
       </c>
-      <c r="L17" s="8">
+      <c r="N17" s="8">
         <v>34010.717452777775</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="4">
         <v>0.6</v>
@@ -2781,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" s="3">
         <v>4</v>
@@ -2790,21 +2908,27 @@
         <v>366.89441874999994</v>
       </c>
       <c r="I18" s="8">
+        <v>19</v>
+      </c>
+      <c r="J18" s="8">
+        <v>79</v>
+      </c>
+      <c r="K18" s="8">
         <v>7338.333333333333</v>
       </c>
-      <c r="J18" s="8">
+      <c r="L18" s="8">
         <v>5283.6402777777776</v>
       </c>
-      <c r="K18" s="8">
+      <c r="M18" s="8">
         <v>16731.527777777777</v>
       </c>
-      <c r="L18" s="8">
+      <c r="N18" s="8">
         <v>29353.50138888889</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4">
         <v>0.52</v>
@@ -2819,7 +2943,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="3">
         <v>4</v>
@@ -2828,21 +2952,27 @@
         <v>289.95980819444441</v>
       </c>
       <c r="I19" s="8">
+        <v>19</v>
+      </c>
+      <c r="J19" s="8">
+        <v>79</v>
+      </c>
+      <c r="K19" s="8">
         <v>6458.8563888888884</v>
       </c>
-      <c r="J19" s="8">
+      <c r="L19" s="8">
         <v>4085.951111111111</v>
       </c>
-      <c r="K19" s="8">
+      <c r="M19" s="8">
         <v>15332.020833333334</v>
       </c>
-      <c r="L19" s="8">
+      <c r="N19" s="8">
         <v>25876.828333333331</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="4">
         <v>0.83</v>
@@ -2857,7 +2987,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="3">
         <v>4</v>
@@ -2866,21 +2996,27 @@
         <v>319.48371291666666</v>
       </c>
       <c r="I20" s="8">
+        <v>19</v>
+      </c>
+      <c r="J20" s="8">
+        <v>79</v>
+      </c>
+      <c r="K20" s="8">
         <v>7797.3772222222224</v>
       </c>
-      <c r="J20" s="8">
+      <c r="L20" s="8">
         <v>5928.2080555555549</v>
       </c>
-      <c r="K20" s="8">
+      <c r="M20" s="8">
         <v>20746.446944444444</v>
       </c>
-      <c r="L20" s="8">
+      <c r="N20" s="8">
         <v>34472.032222222217</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2">
         <v>0.62</v>
@@ -2903,24 +3039,32 @@
       <c r="H21" s="8">
         <v>319.48371291666666</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="8">
+        <v>20</v>
+      </c>
+      <c r="J21" s="8">
+        <v>80</v>
+      </c>
+      <c r="K21" s="3">
         <v>6000</v>
       </c>
-      <c r="J21" s="3">
+      <c r="L21" s="3">
         <v>5000</v>
       </c>
-      <c r="K21" s="3">
+      <c r="M21" s="3">
         <v>17000</v>
       </c>
-      <c r="L21" s="3">
+      <c r="N21" s="3">
         <v>28000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="B22" s="12">
+        <v>0.7</v>
+      </c>
       <c r="C22" s="3">
         <v>3</v>
       </c>
@@ -2939,16 +3083,36 @@
       <c r="H22" s="8">
         <v>319.48371291666666</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="I22" s="8">
+        <v>20</v>
+      </c>
+      <c r="J22" s="8">
+        <v>80</v>
+      </c>
+      <c r="K22" s="8">
+        <f>K10*1.07</f>
+        <v>5879.8754133333341</v>
+      </c>
+      <c r="L22" s="8">
+        <f>L10*1.07</f>
+        <v>3919.916942222223</v>
+      </c>
+      <c r="M22" s="8">
+        <f>M10*1.07</f>
+        <v>14699.688533333334</v>
+      </c>
+      <c r="N22" s="8">
+        <f>N10*1.07</f>
+        <v>24499.480888888895</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.4</v>
+      </c>
       <c r="C23" s="3">
         <v>0</v>
       </c>
@@ -2967,16 +3131,36 @@
       <c r="H23" s="8">
         <v>319.48371291666666</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="I23" s="8">
+        <v>20</v>
+      </c>
+      <c r="J23" s="8">
+        <v>80</v>
+      </c>
+      <c r="K23" s="8">
+        <f t="shared" ref="K23:N25" si="0">K11*1.07</f>
+        <v>4246.9889633611119</v>
+      </c>
+      <c r="L23" s="8">
+        <f t="shared" si="0"/>
+        <v>2831.3259751777778</v>
+      </c>
+      <c r="M23" s="8">
+        <f t="shared" si="0"/>
+        <v>8309.3262315000011</v>
+      </c>
+      <c r="N23" s="8">
+        <f t="shared" si="0"/>
+        <v>15387.641170038891</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="B24" s="12">
+        <v>0.6</v>
+      </c>
       <c r="C24" s="3">
         <v>0</v>
       </c>
@@ -2990,21 +3174,41 @@
         <v>49</v>
       </c>
       <c r="G24" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H24" s="8">
         <v>319.48371291666666</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="I24" s="8">
+        <v>20</v>
+      </c>
+      <c r="J24" s="8">
+        <v>80</v>
+      </c>
+      <c r="K24" s="8">
+        <f t="shared" si="0"/>
+        <v>6073.2555027777771</v>
+      </c>
+      <c r="L24" s="8">
+        <f t="shared" si="0"/>
+        <v>4048.8369027777776</v>
+      </c>
+      <c r="M24" s="8">
+        <f t="shared" si="0"/>
+        <v>15831.990472222224</v>
+      </c>
+      <c r="N24" s="8">
+        <f t="shared" si="0"/>
+        <v>25954.082877777779</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="B25" s="12">
+        <v>0.8</v>
+      </c>
       <c r="C25" s="3">
         <v>5</v>
       </c>
@@ -3018,17 +3222,35 @@
         <v>49</v>
       </c>
       <c r="G25" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H25" s="8">
         <v>319.48371291666666</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I25" s="8">
+        <v>20</v>
+      </c>
+      <c r="J25" s="8">
+        <v>80</v>
+      </c>
+      <c r="K25" s="8">
+        <f t="shared" si="0"/>
+        <v>8771.6144944444441</v>
+      </c>
+      <c r="L25" s="8">
+        <f t="shared" si="0"/>
+        <v>5847.7431944444452</v>
+      </c>
+      <c r="M25" s="8">
+        <f t="shared" si="0"/>
+        <v>17161.85453611111</v>
+      </c>
+      <c r="N25" s="8">
+        <f t="shared" si="0"/>
+        <v>31781.212224999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added seasonality variable to data set
</commit_message>
<xml_diff>
--- a/budgetusd.xlsx
+++ b/budgetusd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielporras/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516FCAF9-6589-FC4F-AE2A-3762CB976694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC23A0AC-B8B2-F548-B156-E804F64A8A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
+    <workbookView xWindow="6380" yWindow="500" windowWidth="18620" windowHeight="13140" activeTab="1" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -177,9 +177,6 @@
     <t>2022-12</t>
   </si>
   <si>
-    <t>Winter North</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -259,6 +256,15 @@
   </si>
   <si>
     <t>Average Price F&amp;B</t>
+  </si>
+  <si>
+    <t>Seasonality</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -726,7 +732,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -2189,7 +2195,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -2214,43 +2220,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>4</v>
@@ -2270,13 +2276,13 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="F2" s="3">
         <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H2" s="3">
         <v>1</v>
@@ -2317,13 +2323,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -2364,13 +2370,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
@@ -2411,13 +2417,13 @@
         <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="3">
         <v>1</v>
@@ -2458,13 +2464,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -2505,13 +2511,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
@@ -2552,13 +2558,13 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F8" s="3">
         <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
@@ -2599,13 +2605,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3">
         <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -2646,13 +2652,13 @@
         <v>3</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
@@ -2693,13 +2699,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
@@ -2740,13 +2746,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="H12" s="3">
         <v>3</v>
@@ -2787,13 +2793,13 @@
         <v>5</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="F13" s="3">
         <v>10</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="3">
         <v>3</v>
@@ -2822,7 +2828,7 @@
     </row>
     <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="4">
         <v>0.81</v>
@@ -2834,13 +2840,13 @@
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="F14" s="3">
         <v>7</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H14" s="3">
         <v>4</v>
@@ -2869,7 +2875,7 @@
     </row>
     <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="4">
         <v>0.82</v>
@@ -2881,13 +2887,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="H15" s="3">
         <v>4</v>
@@ -2916,7 +2922,7 @@
     </row>
     <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="4">
         <v>0.73</v>
@@ -2928,13 +2934,13 @@
         <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="H16" s="3">
         <v>4</v>
@@ -2963,7 +2969,7 @@
     </row>
     <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="4">
         <v>0.78</v>
@@ -2975,13 +2981,13 @@
         <v>5</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="F17" s="3">
         <v>0</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -3010,7 +3016,7 @@
     </row>
     <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4">
         <v>0.6</v>
@@ -3022,13 +3028,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F18" s="3">
         <v>0</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" s="3">
         <v>4</v>
@@ -3057,7 +3063,7 @@
     </row>
     <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="4">
         <v>0.52</v>
@@ -3069,13 +3075,13 @@
         <v>0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="3">
         <v>4</v>
@@ -3104,7 +3110,7 @@
     </row>
     <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4">
         <v>0.83</v>
@@ -3116,13 +3122,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F20" s="3">
         <v>20</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H20" s="3">
         <v>4</v>
@@ -3151,7 +3157,7 @@
     </row>
     <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="2">
         <v>0.62</v>
@@ -3163,13 +3169,13 @@
         <v>2</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F21" s="3">
         <v>10</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H21" s="3">
         <v>4</v>
@@ -3198,7 +3204,7 @@
     </row>
     <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="12">
         <v>0.7</v>
@@ -3210,13 +3216,13 @@
         <v>3</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F22" s="3">
         <v>0</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H22" s="3">
         <v>4</v>
@@ -3247,7 +3253,7 @@
     </row>
     <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="12">
         <v>0.4</v>
@@ -3259,13 +3265,13 @@
         <v>0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F23" s="3">
         <v>0</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H23" s="3">
         <v>4</v>
@@ -3296,7 +3302,7 @@
     </row>
     <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="12">
         <v>0.63</v>
@@ -3308,13 +3314,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="H24" s="3">
         <v>5</v>
@@ -3345,7 +3351,7 @@
     </row>
     <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="12">
         <v>0.84</v>
@@ -3357,13 +3363,13 @@
         <v>5</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="F25" s="3">
         <v>10</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H25" s="3">
         <v>5</v>
@@ -3458,5 +3464,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
applied prediction tests to the model
</commit_message>
<xml_diff>
--- a/budgetusd.xlsx
+++ b/budgetusd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielporras/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091D29CD-A7E7-CA42-A260-DED2A2D40AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F7D517-3BD2-1F4B-BAAB-52018908D147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
+    <workbookView xWindow="-2040" yWindow="740" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -266,6 +266,78 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>2024-01</t>
+  </si>
+  <si>
+    <t>2024-02</t>
+  </si>
+  <si>
+    <t>2024-03</t>
+  </si>
+  <si>
+    <t>2024-04</t>
+  </si>
+  <si>
+    <t>2024-05</t>
+  </si>
+  <si>
+    <t>2024-06</t>
+  </si>
+  <si>
+    <t>2024-07</t>
+  </si>
+  <si>
+    <t>2024-08</t>
+  </si>
+  <si>
+    <t>2024-09</t>
+  </si>
+  <si>
+    <t>2024-10</t>
+  </si>
+  <si>
+    <t>2024-11</t>
+  </si>
+  <si>
+    <t>2024-12</t>
+  </si>
+  <si>
+    <t>2025-01</t>
+  </si>
+  <si>
+    <t>2025-02</t>
+  </si>
+  <si>
+    <t>2025-03</t>
+  </si>
+  <si>
+    <t>2025-04</t>
+  </si>
+  <si>
+    <t>2025-05</t>
+  </si>
+  <si>
+    <t>2025-06</t>
+  </si>
+  <si>
+    <t>2025-07</t>
+  </si>
+  <si>
+    <t>2025-08</t>
+  </si>
+  <si>
+    <t>2025-09</t>
+  </si>
+  <si>
+    <t>2025-10</t>
+  </si>
+  <si>
+    <t>2025-11</t>
+  </si>
+  <si>
+    <t>2025-12</t>
   </si>
 </sst>
 </file>
@@ -275,7 +347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -333,10 +405,60 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -347,7 +469,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -355,12 +477,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -375,7 +512,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,7 +850,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2195,8 +2351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE46400-3D03-3941-9442-654DF1291CF8}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD25"/>
+    <sheetView topLeftCell="G2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -3471,14 +3627,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5970CE32-5E8E-1543-83EC-5C6420665334}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="24" style="15" customWidth="1"/>
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" customWidth="1"/>
@@ -3489,888 +3647,2004 @@
     <col min="9" max="9" width="24.83203125" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
     <col min="11" max="11" width="28.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" customWidth="1"/>
+    <col min="17" max="19" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="31"/>
+    </row>
+    <row r="2" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="31">
+        <v>0</v>
+      </c>
+      <c r="C2" s="31">
+        <v>0</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="31">
+        <v>0</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="31">
+        <v>1</v>
+      </c>
+      <c r="H2" s="31">
+        <v>10</v>
+      </c>
+      <c r="I2" s="31">
+        <v>70</v>
+      </c>
+      <c r="J2" s="31">
+        <v>9</v>
+      </c>
+      <c r="K2" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="31">
+        <v>0</v>
+      </c>
+      <c r="C3" s="31">
+        <v>0</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="31">
+        <v>0</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="31">
+        <v>1</v>
+      </c>
+      <c r="H3" s="31">
+        <v>10</v>
+      </c>
+      <c r="I3" s="31">
+        <v>70</v>
+      </c>
+      <c r="J3" s="31">
+        <v>9</v>
+      </c>
+      <c r="K3" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="31">
+        <v>0</v>
+      </c>
+      <c r="C4" s="31">
+        <v>0</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="31">
+        <v>0</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="31">
+        <v>1</v>
+      </c>
+      <c r="H4" s="31">
+        <v>10</v>
+      </c>
+      <c r="I4" s="31">
+        <v>70</v>
+      </c>
+      <c r="J4" s="31">
+        <v>9</v>
+      </c>
+      <c r="K4" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B5" s="18">
         <v>0.61</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C5" s="19">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D5" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E5" s="19">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G5" s="19">
         <v>1</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H5" s="20">
         <v>62.111111111111114</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I5" s="20">
         <v>75</v>
       </c>
-      <c r="J2" s="8">
-        <v>9</v>
-      </c>
-      <c r="K2" s="8">
+      <c r="J5" s="20">
+        <v>9</v>
+      </c>
+      <c r="K5" s="20">
         <v>13136.888888888889</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+    </row>
+    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B6" s="18">
         <v>0.62</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C6" s="19">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D6" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E6" s="19">
+        <v>0</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G6" s="19">
         <v>1</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H6" s="20">
         <v>62.111111111111114</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I6" s="20">
         <v>75</v>
       </c>
-      <c r="J3" s="8">
-        <v>9</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="J6" s="20">
+        <v>9</v>
+      </c>
+      <c r="K6" s="20">
         <v>11430.527777777777</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+    </row>
+    <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B7" s="18">
         <v>0.39</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C7" s="19">
+        <v>0</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E7" s="19">
+        <v>0</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G7" s="19">
         <v>1</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H7" s="20">
         <v>99.305555555555557</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I7" s="20">
         <v>75</v>
       </c>
-      <c r="J4" s="8">
-        <v>9</v>
-      </c>
-      <c r="K4" s="8">
+      <c r="J7" s="20">
+        <v>9</v>
+      </c>
+      <c r="K7" s="20">
         <v>9742.6111111111113</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+    </row>
+    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B8" s="18">
         <v>0.7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C8" s="19">
         <v>5</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D8" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E8" s="19">
+        <v>0</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G8" s="19">
         <v>1</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H8" s="20">
         <v>246.05555555555554</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I8" s="20">
         <v>75</v>
       </c>
-      <c r="J5" s="8">
-        <v>9</v>
-      </c>
-      <c r="K5" s="8">
+      <c r="J8" s="20">
+        <v>9</v>
+      </c>
+      <c r="K8" s="20">
         <v>15043.805555555555</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+    </row>
+    <row r="9" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B9" s="18">
         <v>0.47</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C9" s="19">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D9" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E9" s="19">
+        <v>0</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G9" s="19">
         <v>1</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H9" s="20">
         <v>144.92038888888888</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I9" s="20">
         <v>75</v>
       </c>
-      <c r="J6" s="8">
-        <v>9</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="J9" s="20">
+        <v>9</v>
+      </c>
+      <c r="K9" s="20">
         <v>8546.1691666666666</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+    </row>
+    <row r="10" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B10" s="18">
         <v>0.33</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C10" s="19">
+        <v>0</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E10" s="19">
+        <v>0</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G10" s="19">
         <v>1</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H10" s="20">
         <v>118.45822222222222</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I10" s="20">
         <v>75</v>
       </c>
-      <c r="J7" s="8">
-        <v>9</v>
-      </c>
-      <c r="K7" s="8">
+      <c r="J10" s="20">
+        <v>9</v>
+      </c>
+      <c r="K10" s="20">
         <v>7171.4191666666666</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+    </row>
+    <row r="11" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B11" s="18">
         <v>0.67</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C11" s="19">
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D11" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E11" s="19">
         <v>20</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F11" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G11" s="19">
         <v>1</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H11" s="20">
         <v>46.761375416666667</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I11" s="20">
         <v>75</v>
       </c>
-      <c r="J8" s="8">
-        <v>9</v>
-      </c>
-      <c r="K8" s="8">
+      <c r="J11" s="20">
+        <v>9</v>
+      </c>
+      <c r="K11" s="20">
         <v>15864.97388888889</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+    </row>
+    <row r="12" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B12" s="18">
         <v>0.49</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C12" s="19">
         <v>2</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D12" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E12" s="19">
         <v>10</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F12" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G12" s="19">
         <v>1</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H12" s="20">
         <v>149.96791666666667</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I12" s="20">
         <v>77</v>
       </c>
-      <c r="J9" s="8">
-        <v>9</v>
-      </c>
-      <c r="K9" s="8">
+      <c r="J12" s="20">
+        <v>9</v>
+      </c>
+      <c r="K12" s="20">
         <v>11925.820833333333</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+    </row>
+    <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B13" s="18">
         <v>0.51</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C13" s="19">
         <v>3</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D13" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="E13" s="19">
+        <v>0</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G13" s="19">
         <v>1</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H13" s="20">
         <v>170.24083333333334</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I13" s="20">
         <v>77</v>
       </c>
-      <c r="J10" s="8">
-        <v>9</v>
-      </c>
-      <c r="K10" s="8">
+      <c r="J13" s="20">
+        <v>9</v>
+      </c>
+      <c r="K13" s="20">
         <v>13738.026666666667</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+    </row>
+    <row r="14" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B14" s="18">
         <v>0.4</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C14" s="19">
+        <v>0</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E14" s="19">
+        <v>0</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G14" s="19">
         <v>1</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H14" s="20">
         <v>176.07463058333332</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I14" s="20">
         <v>77</v>
       </c>
-      <c r="J11" s="8">
-        <v>9</v>
-      </c>
-      <c r="K11" s="8">
+      <c r="J14" s="20">
+        <v>9</v>
+      </c>
+      <c r="K14" s="20">
         <v>7765.7254499999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+    </row>
+    <row r="15" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B15" s="18">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C15" s="19">
+        <v>0</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="E15" s="19">
+        <v>0</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G15" s="19">
         <v>3</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H15" s="20">
         <v>176.07463058333332</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I15" s="20">
         <v>77</v>
       </c>
-      <c r="J12" s="8">
-        <v>9</v>
-      </c>
-      <c r="K12" s="8">
+      <c r="J15" s="20">
+        <v>9</v>
+      </c>
+      <c r="K15" s="20">
         <v>14796.252777777778</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+    </row>
+    <row r="16" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B16" s="18">
         <v>0.79</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C16" s="19">
         <v>5</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D16" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E16" s="19">
         <v>10</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F16" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G16" s="19">
         <v>3</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H16" s="20">
         <v>196.63585922222222</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I16" s="20">
         <v>77</v>
       </c>
-      <c r="J13" s="8">
-        <v>9</v>
-      </c>
-      <c r="K13" s="8">
+      <c r="J16" s="20">
+        <v>9</v>
+      </c>
+      <c r="K16" s="20">
         <v>16039.116388888888</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+    </row>
+    <row r="17" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B17" s="18">
         <v>0.81</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C17" s="19">
         <v>3</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D17" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E17" s="19">
         <v>7</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F17" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G17" s="19">
         <v>4</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H17" s="20">
         <v>277.43523555555555</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I17" s="20">
         <v>80</v>
       </c>
-      <c r="J14" s="8">
-        <v>9</v>
-      </c>
-      <c r="K14" s="8">
+      <c r="J17" s="20">
+        <v>9</v>
+      </c>
+      <c r="K17" s="20">
         <v>18609.989444444444</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="L17" s="32"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="31"/>
+    </row>
+    <row r="18" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B18" s="18">
         <v>0.82</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C18" s="19">
         <v>1</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D18" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="E18" s="19">
+        <v>0</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G18" s="19">
         <v>4</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H18" s="20">
         <v>583.33333333333337</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I18" s="20">
         <v>80</v>
       </c>
-      <c r="J15" s="8">
-        <v>9</v>
-      </c>
-      <c r="K15" s="8">
+      <c r="J18" s="20">
+        <v>9</v>
+      </c>
+      <c r="K18" s="20">
         <v>16622.081111111111</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="L18" s="32"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+    </row>
+    <row r="19" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B19" s="18">
+        <v>0.78</v>
+      </c>
+      <c r="C19" s="19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="19">
+        <v>4</v>
+      </c>
+      <c r="H19" s="20">
+        <v>189.90263766666666</v>
+      </c>
+      <c r="I19" s="20">
+        <v>83</v>
+      </c>
+      <c r="J19" s="20">
+        <v>9</v>
+      </c>
+      <c r="K19" s="20">
+        <v>21306.423360019777</v>
+      </c>
+      <c r="L19" s="32"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+    </row>
+    <row r="20" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="18">
         <v>0.73</v>
       </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C20" s="19">
+        <v>5</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="E20" s="19">
+        <v>0</v>
+      </c>
+      <c r="F20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G20" s="19">
         <v>4</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H20" s="20">
+        <v>339.38964222222216</v>
+      </c>
+      <c r="I20" s="20">
+        <v>80</v>
+      </c>
+      <c r="J20" s="20">
+        <v>9</v>
+      </c>
+      <c r="K20" s="20">
+        <v>17039.369466666667</v>
+      </c>
+      <c r="L20" s="32"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+    </row>
+    <row r="21" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="C21" s="19">
+        <v>1</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="19">
+        <v>0</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="19">
+        <v>4</v>
+      </c>
+      <c r="H21" s="20">
+        <v>366.89441874999994</v>
+      </c>
+      <c r="I21" s="20">
+        <v>80</v>
+      </c>
+      <c r="J21" s="20">
+        <v>9</v>
+      </c>
+      <c r="K21" s="20">
+        <v>16731.527777777777</v>
+      </c>
+      <c r="L21" s="32"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+    </row>
+    <row r="22" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="18">
+        <v>0.52</v>
+      </c>
+      <c r="C22" s="19">
+        <v>0</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="19">
+        <v>0</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="19">
+        <v>4</v>
+      </c>
+      <c r="H22" s="20">
+        <v>289.95980819444441</v>
+      </c>
+      <c r="I22" s="20">
+        <v>80</v>
+      </c>
+      <c r="J22" s="20">
+        <v>9</v>
+      </c>
+      <c r="K22" s="20">
+        <v>15332.020833333334</v>
+      </c>
+      <c r="L22" s="32"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+    </row>
+    <row r="23" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="18">
+        <v>0.83</v>
+      </c>
+      <c r="C23" s="19">
+        <v>3</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="19">
+        <v>20</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="19">
+        <v>4</v>
+      </c>
+      <c r="H23" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I23" s="20">
+        <v>80</v>
+      </c>
+      <c r="J23" s="20">
+        <v>9</v>
+      </c>
+      <c r="K23" s="20">
+        <v>20746.446944444444</v>
+      </c>
+      <c r="L23" s="32"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+    </row>
+    <row r="24" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="21">
+        <v>0.62</v>
+      </c>
+      <c r="C24" s="19">
+        <v>2</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="19">
+        <v>10</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="19">
+        <v>4</v>
+      </c>
+      <c r="H24" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I24" s="20">
+        <v>84</v>
+      </c>
+      <c r="J24" s="20">
+        <v>9</v>
+      </c>
+      <c r="K24" s="19">
+        <v>17000</v>
+      </c>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+    </row>
+    <row r="25" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="C25" s="19">
+        <v>3</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="19">
+        <v>0</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="19">
+        <v>4</v>
+      </c>
+      <c r="H25" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I25" s="20">
+        <v>84</v>
+      </c>
+      <c r="J25" s="20">
+        <v>9</v>
+      </c>
+      <c r="K25" s="20">
+        <f>K13*1.07</f>
+        <v>14699.688533333334</v>
+      </c>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+    </row>
+    <row r="26" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A26" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="C26" s="19">
+        <v>0</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="19">
+        <v>0</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="19">
+        <v>4</v>
+      </c>
+      <c r="H26" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I26" s="20">
+        <v>84</v>
+      </c>
+      <c r="J26" s="20">
+        <v>9</v>
+      </c>
+      <c r="K26" s="20">
+        <f>K14*1.07</f>
+        <v>8309.3262315000011</v>
+      </c>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+    </row>
+    <row r="27" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="22">
+        <v>0.63</v>
+      </c>
+      <c r="C27" s="19">
+        <v>0</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="19">
+        <v>0</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="19">
+        <v>5</v>
+      </c>
+      <c r="H27" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I27" s="20">
+        <v>84</v>
+      </c>
+      <c r="J27" s="20">
+        <v>9</v>
+      </c>
+      <c r="K27" s="20">
+        <f>K15*1.1</f>
+        <v>16275.878055555557</v>
+      </c>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+    </row>
+    <row r="28" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A28" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="22">
+        <v>0.84</v>
+      </c>
+      <c r="C28" s="19">
+        <v>5</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="19">
+        <v>10</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="19">
+        <v>5</v>
+      </c>
+      <c r="H28" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I28" s="20">
+        <v>84</v>
+      </c>
+      <c r="J28" s="20">
+        <v>9</v>
+      </c>
+      <c r="K28" s="20">
+        <f>K16*1.1</f>
+        <v>17643.028027777778</v>
+      </c>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+    </row>
+    <row r="29" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A29" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="23">
+        <v>0.83</v>
+      </c>
+      <c r="C29" s="19">
+        <v>3</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="19">
+        <v>7</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="19">
+        <v>4</v>
+      </c>
+      <c r="H29" s="20">
+        <v>277.43523555555555</v>
+      </c>
+      <c r="I29" s="20">
+        <v>85</v>
+      </c>
+      <c r="J29" s="20">
+        <v>9</v>
+      </c>
+      <c r="K29" s="20">
+        <f>(B29*K17)/B17</f>
+        <v>19069.495356652948</v>
+      </c>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+    </row>
+    <row r="30" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A30" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="23">
+        <v>0.84</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="19">
+        <v>0</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" s="19">
+        <v>4</v>
+      </c>
+      <c r="H30" s="20">
+        <v>583.33333333333337</v>
+      </c>
+      <c r="I30" s="20">
+        <v>85</v>
+      </c>
+      <c r="J30" s="20">
+        <v>9</v>
+      </c>
+      <c r="K30" s="20">
+        <f>(B30*K18)/B18</f>
+        <v>17027.497723577235</v>
+      </c>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+    </row>
+    <row r="31" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A31" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="C31" s="19">
+        <v>0</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="19">
+        <v>0</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="19">
+        <v>4</v>
+      </c>
+      <c r="H31" s="20">
         <v>189.90263766666666</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I31" s="20">
+        <v>85</v>
+      </c>
+      <c r="J31" s="20">
+        <v>9</v>
+      </c>
+      <c r="K31" s="20">
+        <f>(B31*K19)/B19</f>
+        <v>20486.945538480555</v>
+      </c>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+    </row>
+    <row r="32" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A32" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="18">
+        <v>0.78</v>
+      </c>
+      <c r="C32" s="19">
+        <v>5</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="19">
+        <v>0</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="19">
+        <v>4</v>
+      </c>
+      <c r="H32" s="20">
+        <v>339.38964222222216</v>
+      </c>
+      <c r="I32" s="20">
+        <v>85</v>
+      </c>
+      <c r="J32" s="20">
+        <v>9</v>
+      </c>
+      <c r="K32" s="20">
+        <v>17039.369466666667</v>
+      </c>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+    </row>
+    <row r="33" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A33" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="J16" s="8">
-        <v>9</v>
-      </c>
-      <c r="K16" s="8">
-        <v>21306.423360019777</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="4">
+      <c r="B33" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="C33" s="19">
+        <v>1</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="19">
+        <v>0</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="19">
+        <v>4</v>
+      </c>
+      <c r="H33" s="20">
+        <v>366.89441874999994</v>
+      </c>
+      <c r="I33" s="20">
+        <v>85</v>
+      </c>
+      <c r="J33" s="20">
+        <v>9</v>
+      </c>
+      <c r="K33" s="20">
+        <v>16731.527777777777</v>
+      </c>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+    </row>
+    <row r="34" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A34" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="23">
+        <v>0.54</v>
+      </c>
+      <c r="C34" s="19">
+        <v>0</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="19">
+        <v>0</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="19">
+        <v>4</v>
+      </c>
+      <c r="H34" s="20">
+        <v>289.95980819444441</v>
+      </c>
+      <c r="I34" s="20">
+        <v>85</v>
+      </c>
+      <c r="J34" s="20">
+        <v>9</v>
+      </c>
+      <c r="K34" s="20">
+        <v>15332.020833333334</v>
+      </c>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+    </row>
+    <row r="35" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A35" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="18">
+        <v>0.83</v>
+      </c>
+      <c r="C35" s="19">
+        <v>3</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="19">
+        <v>20</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="19">
+        <v>4</v>
+      </c>
+      <c r="H35" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I35" s="20">
+        <v>85</v>
+      </c>
+      <c r="J35" s="20">
+        <v>9</v>
+      </c>
+      <c r="K35" s="20">
+        <v>20746.446944444444</v>
+      </c>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+    </row>
+    <row r="36" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A36" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="21">
+        <v>0.62</v>
+      </c>
+      <c r="C36" s="19">
+        <v>2</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="19">
+        <v>10</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="19">
+        <v>4</v>
+      </c>
+      <c r="H36" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I36" s="20">
+        <v>85</v>
+      </c>
+      <c r="J36" s="20">
+        <v>9</v>
+      </c>
+      <c r="K36" s="19">
+        <v>17000</v>
+      </c>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+    </row>
+    <row r="37" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A37" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="C37" s="19">
+        <v>3</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="19">
+        <v>0</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="19">
+        <v>4</v>
+      </c>
+      <c r="H37" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I37" s="20">
+        <v>85</v>
+      </c>
+      <c r="J37" s="20">
+        <v>9</v>
+      </c>
+      <c r="K37" s="20">
+        <f>K25*1.07</f>
+        <v>15728.666730666668</v>
+      </c>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+    </row>
+    <row r="38" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A38" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="C38" s="19">
+        <v>0</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" s="19">
+        <v>0</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="19">
+        <v>4</v>
+      </c>
+      <c r="H38" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I38" s="20">
+        <v>85</v>
+      </c>
+      <c r="J38" s="20">
+        <v>9</v>
+      </c>
+      <c r="K38" s="20">
+        <f>K26*1.07</f>
+        <v>8890.9790677050023</v>
+      </c>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+    </row>
+    <row r="39" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A39" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="24">
+        <v>0.65</v>
+      </c>
+      <c r="C39" s="19">
+        <v>0</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="19">
+        <v>0</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="19">
+        <v>5</v>
+      </c>
+      <c r="H39" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I39" s="20">
+        <v>86</v>
+      </c>
+      <c r="J39" s="20">
+        <v>9</v>
+      </c>
+      <c r="K39" s="20">
+        <f>(B39*K27)/B27</f>
+        <v>16792.572597001767</v>
+      </c>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+    </row>
+    <row r="40" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A40" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="24">
+        <v>0.86</v>
+      </c>
+      <c r="C40" s="19">
+        <v>5</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="19">
+        <v>10</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="19">
+        <v>5</v>
+      </c>
+      <c r="H40" s="20">
+        <v>319.48371291666666</v>
+      </c>
+      <c r="I40" s="20">
+        <v>86</v>
+      </c>
+      <c r="J40" s="20">
+        <v>9</v>
+      </c>
+      <c r="K40" s="20">
+        <f t="shared" ref="K40:K52" si="0">(B40*K28)/B28</f>
+        <v>18063.10012367725</v>
+      </c>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+    </row>
+    <row r="41" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A41" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="C41" s="19">
+        <v>3</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" s="19">
+        <v>7</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" s="19">
+        <v>4</v>
+      </c>
+      <c r="H41" s="20">
+        <v>277.43523555555555</v>
+      </c>
+      <c r="I41" s="20">
+        <v>86</v>
+      </c>
+      <c r="J41" s="20">
+        <v>9</v>
+      </c>
+      <c r="K41" s="20">
+        <f t="shared" si="0"/>
+        <v>19758.754224965702</v>
+      </c>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+    </row>
+    <row r="42" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A42" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="25">
+        <v>0.87</v>
+      </c>
+      <c r="C42" s="19">
+        <v>1</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="19">
+        <v>0</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="19">
+        <v>4</v>
+      </c>
+      <c r="H42" s="20">
+        <v>583.33333333333337</v>
+      </c>
+      <c r="I42" s="20">
+        <v>86</v>
+      </c>
+      <c r="J42" s="20">
+        <v>9</v>
+      </c>
+      <c r="K42" s="20">
+        <f t="shared" si="0"/>
+        <v>17635.622642276423</v>
+      </c>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+    </row>
+    <row r="43" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A43" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="25">
         <v>0.78</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C43" s="19">
+        <v>0</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="19">
+        <v>0</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="19">
+        <v>4</v>
+      </c>
+      <c r="H43" s="20">
+        <v>189.90263766666666</v>
+      </c>
+      <c r="I43" s="20">
+        <v>86</v>
+      </c>
+      <c r="J43" s="20">
+        <v>9</v>
+      </c>
+      <c r="K43" s="20">
+        <f t="shared" si="0"/>
+        <v>21306.42336001978</v>
+      </c>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+    </row>
+    <row r="44" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A44" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="26">
+        <v>0.78</v>
+      </c>
+      <c r="C44" s="19">
         <v>5</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D44" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="E44" s="19">
+        <v>0</v>
+      </c>
+      <c r="F44" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G44" s="19">
         <v>4</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H44" s="20">
         <v>339.38964222222216</v>
       </c>
-      <c r="I17" s="8">
-        <v>80</v>
-      </c>
-      <c r="J17" s="8">
-        <v>9</v>
-      </c>
-      <c r="K17" s="8">
+      <c r="I44" s="20">
+        <v>86</v>
+      </c>
+      <c r="J44" s="20">
+        <v>9</v>
+      </c>
+      <c r="K44" s="20">
+        <f t="shared" si="0"/>
         <v>17039.369466666667</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
+    </row>
+    <row r="45" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A45" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="26">
         <v>0.6</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C45" s="19">
         <v>1</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D45" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="E45" s="19">
+        <v>0</v>
+      </c>
+      <c r="F45" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G45" s="19">
         <v>4</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H45" s="20">
         <v>366.89441874999994</v>
       </c>
-      <c r="I18" s="8">
-        <v>80</v>
-      </c>
-      <c r="J18" s="8">
-        <v>9</v>
-      </c>
-      <c r="K18" s="8">
-        <v>16731.527777777777</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="4">
-        <v>0.52</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="I45" s="20">
+        <v>86</v>
+      </c>
+      <c r="J45" s="20">
+        <v>9</v>
+      </c>
+      <c r="K45" s="20">
+        <f>(B45*K49)/B48</f>
+        <v>15221.290384516129</v>
+      </c>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+      <c r="N45" s="31"/>
+    </row>
+    <row r="46" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A46" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="25">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C46" s="19">
+        <v>0</v>
+      </c>
+      <c r="D46" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="E46" s="19">
+        <v>0</v>
+      </c>
+      <c r="F46" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G46" s="19">
         <v>4</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H46" s="20">
         <v>289.95980819444441</v>
       </c>
-      <c r="I19" s="8">
-        <v>80</v>
-      </c>
-      <c r="J19" s="8">
-        <v>9</v>
-      </c>
-      <c r="K19" s="8">
-        <v>15332.020833333334</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="I46" s="20">
+        <v>86</v>
+      </c>
+      <c r="J46" s="20">
+        <v>9</v>
+      </c>
+      <c r="K46" s="20">
+        <f>(B46*K45)/B45</f>
+        <v>14460.225865290322</v>
+      </c>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+    </row>
+    <row r="47" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A47" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="26">
         <v>0.83</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C47" s="19">
         <v>3</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D47" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E47" s="19">
         <v>20</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F47" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G47" s="19">
         <v>4</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H47" s="20">
         <v>319.48371291666666</v>
       </c>
-      <c r="I20" s="8">
-        <v>80</v>
-      </c>
-      <c r="J20" s="8">
-        <v>9</v>
-      </c>
-      <c r="K20" s="8">
+      <c r="I47" s="20">
+        <v>86</v>
+      </c>
+      <c r="J47" s="20">
+        <v>9</v>
+      </c>
+      <c r="K47" s="20">
+        <f t="shared" si="0"/>
         <v>20746.446944444444</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="2">
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+    </row>
+    <row r="48" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A48" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="21">
         <v>0.62</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C48" s="19">
         <v>2</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D48" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E48" s="19">
         <v>10</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F48" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G48" s="19">
         <v>4</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H48" s="20">
         <v>319.48371291666666</v>
       </c>
-      <c r="I21" s="8">
-        <v>84</v>
-      </c>
-      <c r="J21" s="8">
-        <v>9</v>
-      </c>
-      <c r="K21" s="3">
+      <c r="I48" s="20">
+        <v>86</v>
+      </c>
+      <c r="J48" s="20">
+        <v>9</v>
+      </c>
+      <c r="K48" s="20">
+        <f t="shared" si="0"/>
         <v>17000</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="12">
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+    </row>
+    <row r="49" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A49" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="27">
         <v>0.7</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C49" s="19">
         <v>3</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D49" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="E49" s="19">
+        <v>0</v>
+      </c>
+      <c r="F49" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G49" s="19">
         <v>4</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H49" s="20">
         <v>319.48371291666666</v>
       </c>
-      <c r="I22" s="8">
-        <v>84</v>
-      </c>
-      <c r="J22" s="8">
-        <v>9</v>
-      </c>
-      <c r="K22" s="8">
-        <f>K10*1.07</f>
-        <v>14699.688533333334</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="12">
+      <c r="I49" s="20">
+        <v>86</v>
+      </c>
+      <c r="J49" s="20">
+        <v>9</v>
+      </c>
+      <c r="K49" s="20">
+        <f t="shared" si="0"/>
+        <v>15728.666730666668</v>
+      </c>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+    </row>
+    <row r="50" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A50" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="27">
         <v>0.4</v>
       </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C50" s="19">
+        <v>0</v>
+      </c>
+      <c r="D50" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="E50" s="19">
+        <v>0</v>
+      </c>
+      <c r="F50" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G50" s="19">
         <v>4</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H50" s="20">
         <v>319.48371291666666</v>
       </c>
-      <c r="I23" s="8">
-        <v>84</v>
-      </c>
-      <c r="J23" s="8">
-        <v>9</v>
-      </c>
-      <c r="K23" s="8">
-        <f>K11*1.07</f>
-        <v>8309.3262315000011</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="12">
-        <v>0.63</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="I50" s="20">
+        <v>86</v>
+      </c>
+      <c r="J50" s="20">
+        <v>9</v>
+      </c>
+      <c r="K50" s="20">
+        <f t="shared" si="0"/>
+        <v>8890.9790677050023</v>
+      </c>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="31"/>
+    </row>
+    <row r="51" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A51" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="28">
+        <v>0.68</v>
+      </c>
+      <c r="C51" s="19">
+        <v>0</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="E51" s="19">
+        <v>0</v>
+      </c>
+      <c r="F51" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G51" s="19">
         <v>5</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H51" s="20">
         <v>319.48371291666666</v>
       </c>
-      <c r="I24" s="8">
-        <v>84</v>
-      </c>
-      <c r="J24" s="8">
-        <v>9</v>
-      </c>
-      <c r="K24" s="8">
-        <f>K12*1.1</f>
-        <v>16275.878055555557</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="12">
-        <v>0.84</v>
-      </c>
-      <c r="C25" s="3">
+      <c r="I51" s="20">
+        <v>87</v>
+      </c>
+      <c r="J51" s="20">
+        <v>9</v>
+      </c>
+      <c r="K51" s="20">
+        <f>(B51*K50)/B50</f>
+        <v>15114.664415098505</v>
+      </c>
+      <c r="L51" s="31"/>
+      <c r="M51" s="31"/>
+      <c r="N51" s="31"/>
+    </row>
+    <row r="52" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="A52" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="28">
+        <v>0.89</v>
+      </c>
+      <c r="C52" s="19">
         <v>5</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D52" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E52" s="19">
         <v>10</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F52" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G52" s="19">
         <v>5</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H52" s="20">
         <v>319.48371291666666</v>
       </c>
-      <c r="I25" s="8">
-        <v>84</v>
-      </c>
-      <c r="J25" s="8">
-        <v>9</v>
-      </c>
-      <c r="K25" s="8">
-        <f>K13*1.1</f>
-        <v>17643.028027777778</v>
-      </c>
+      <c r="I52" s="20">
+        <v>87</v>
+      </c>
+      <c r="J52" s="20">
+        <v>9</v>
+      </c>
+      <c r="K52" s="20">
+        <f t="shared" si="0"/>
+        <v>18693.208267526457</v>
+      </c>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="31"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tested pygwalker on jupyter notebook
</commit_message>
<xml_diff>
--- a/budgetusd.xlsx
+++ b/budgetusd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielporras/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628A2BBD-8CBE-4B45-99B8-DBADB291ED91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A77EAA-37EE-F045-83C3-719AB675A462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
+    <workbookView xWindow="-2120" yWindow="580" windowWidth="28800" windowHeight="15840" activeTab="5" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -14173,7 +14173,7 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD49"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cleaned and saved expenses model
</commit_message>
<xml_diff>
--- a/budgetusd.xlsx
+++ b/budgetusd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielporras/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6975449-B67A-CB45-BF88-5B323F8657BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAB635C-840C-1448-AB6E-21DEA0876869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="3" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
+    <workbookView xWindow="100" yWindow="640" windowWidth="27480" windowHeight="15840" activeTab="7" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="112">
   <si>
     <t>Date</t>
   </si>
@@ -369,6 +369,18 @@
   <si>
     <t>Total Indirect Costs</t>
   </si>
+  <si>
+    <t>201-10</t>
+  </si>
+  <si>
+    <t>2021-11</t>
+  </si>
+  <si>
+    <t>2021-12</t>
+  </si>
+  <si>
+    <t>Rooms Cost</t>
+  </si>
 </sst>
 </file>
 
@@ -378,7 +390,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="mmm/yyyy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -527,6 +539,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -577,7 +610,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -645,6 +678,13 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -3744,8 +3784,8 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3801,7 +3841,7 @@
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="B2" s="34">
         <v>0</v>
@@ -3836,7 +3876,7 @@
     </row>
     <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
@@ -3871,7 +3911,7 @@
     </row>
     <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="B4" s="34">
         <v>0</v>
@@ -5617,8 +5657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3125D8-EE63-4B43-9AC6-51D16219A8B2}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13939,8 +13979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD220802-990C-0943-A7BD-ACE19BFC12F7}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -15118,14 +15158,14 @@
         <v>762.77981426611791</v>
       </c>
       <c r="L26" s="28">
-        <v>277.43523555555555</v>
+        <v>277.43523555555601</v>
       </c>
       <c r="M26" s="28">
         <v>1072.9548177829217</v>
       </c>
       <c r="N26" s="59">
         <f t="shared" si="0"/>
-        <v>14819.625331381891</v>
+        <v>14819.625331381892</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -16171,819 +16211,1043 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B880BA27-03E5-754E-A602-A8FF5ACB6DE8}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B49"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="55"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="56">
         <v>43831</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="32">
+        <v>0.61</v>
+      </c>
+      <c r="C2" s="28">
         <v>11744.194444444445</v>
       </c>
-      <c r="C2" s="28">
+      <c r="D2" s="28">
         <v>5247.9444444444443</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="56">
         <v>43862</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="32">
+        <v>0.62</v>
+      </c>
+      <c r="C3" s="28">
         <v>9433.3333333333339</v>
       </c>
-      <c r="C3" s="28">
+      <c r="D3" s="28">
         <v>5794.6388888888887</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="56">
         <v>43891</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="32">
+        <v>0.39</v>
+      </c>
+      <c r="C4" s="28">
         <v>8833.0833333333339</v>
       </c>
-      <c r="C4" s="28">
+      <c r="D4" s="28">
         <v>4194.4444444444443</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="56">
         <v>43922</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="C5" s="28">
         <v>18834.583333333332</v>
       </c>
-      <c r="C5" s="28">
+      <c r="D5" s="28">
         <v>7372.1388888888887</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="56">
         <v>43952</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="32">
+        <v>0.47</v>
+      </c>
+      <c r="C6" s="28">
         <v>9258.3499999999985</v>
       </c>
-      <c r="C6" s="28">
+      <c r="D6" s="28">
         <v>3003.0014884777779</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="56">
         <v>43983</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="32">
+        <v>0.33</v>
+      </c>
+      <c r="C7" s="28">
         <v>4703.32</v>
       </c>
-      <c r="C7" s="28">
+      <c r="D7" s="28">
         <v>1722.2222222222222</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="56">
         <v>44013</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="32">
+        <v>0.67</v>
+      </c>
+      <c r="C8" s="28">
         <v>10576.649166666666</v>
       </c>
-      <c r="C8" s="28">
+      <c r="D8" s="28">
         <v>3995.7875000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="56">
         <v>44044</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="32">
+        <v>0.49</v>
+      </c>
+      <c r="C9" s="28">
         <v>8996.6717500000013</v>
       </c>
-      <c r="C9" s="28">
+      <c r="D9" s="28">
         <v>3067.4377222209996</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="56">
         <v>44075</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="32">
+        <v>0.51</v>
+      </c>
+      <c r="C10" s="28">
         <v>9158.684444444445</v>
       </c>
-      <c r="C10" s="28">
+      <c r="D10" s="28">
         <v>3947.0252281785552</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="56">
         <v>44105</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="C11" s="28">
         <v>6615.247606111112</v>
       </c>
-      <c r="C11" s="28">
+      <c r="D11" s="28">
         <v>2060.161106686664</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="56">
         <v>44136</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="32">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C12" s="28">
         <v>9459.8994444444434</v>
       </c>
-      <c r="C12" s="28">
+      <c r="D12" s="28">
         <v>3896.0550900333333</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="56">
         <v>44166</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="32">
+        <v>0.79</v>
+      </c>
+      <c r="C13" s="28">
         <v>13662.95111111111</v>
       </c>
-      <c r="C13" s="28">
+      <c r="D13" s="28">
         <v>6203.3228744444441</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="56">
         <v>44197</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="32">
+        <v>0.81</v>
+      </c>
+      <c r="C14" s="28">
         <v>16288.453888888889</v>
       </c>
-      <c r="C14" s="28">
+      <c r="D14" s="28">
         <v>6396.799722222222</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="56">
         <v>44228</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="32">
+        <v>0.82</v>
+      </c>
+      <c r="C15" s="28">
         <v>10187.727061111113</v>
       </c>
-      <c r="C15" s="28">
+      <c r="D15" s="28">
         <v>4136.1069444444447</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="56">
         <v>44256</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="32">
+        <v>0.78</v>
+      </c>
+      <c r="C16" s="28">
         <v>13240.710251091332</v>
       </c>
-      <c r="C16" s="28">
+      <c r="D16" s="28">
         <v>5017.6605555555561</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="56">
         <v>44287</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="32">
+        <v>0.73</v>
+      </c>
+      <c r="C17" s="28">
         <v>16971.347986111112</v>
       </c>
-      <c r="C17" s="28">
+      <c r="D17" s="28">
         <v>7282.2305833333339</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="56">
         <v>44317</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="C18" s="28">
         <v>12621.973611111111</v>
       </c>
-      <c r="C18" s="28">
+      <c r="D18" s="28">
         <v>4708.2878916666668</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="56">
         <v>44348</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="32">
+        <v>0.52</v>
+      </c>
+      <c r="C19" s="28">
         <v>10544.807499999999</v>
       </c>
-      <c r="C19" s="28">
+      <c r="D19" s="28">
         <v>4511.0556569444443</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="56">
         <v>44378</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="32">
+        <v>0.83</v>
+      </c>
+      <c r="C20" s="28">
         <v>13725.585277777776</v>
       </c>
-      <c r="C20" s="28">
+      <c r="D20" s="28">
         <v>5402.806863888889</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="56">
         <v>44409</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="32">
+        <v>0.62</v>
+      </c>
+      <c r="C21" s="28">
         <v>11000</v>
       </c>
-      <c r="C21" s="28">
+      <c r="D21" s="28">
         <v>4290</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="56">
         <v>44440</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="C22" s="28">
         <v>9799.7923555555572</v>
       </c>
-      <c r="C22" s="28">
+      <c r="D22" s="28">
         <v>3821.9190186666674</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="56">
         <v>44470</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="C23" s="28">
         <v>7078.3149385388897</v>
       </c>
-      <c r="C23" s="28">
+      <c r="D23" s="28">
         <v>2760.5428260301669</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="56">
         <v>44501</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="32">
+        <v>0.63</v>
+      </c>
+      <c r="C24" s="28">
         <v>10405.889388888889</v>
       </c>
-      <c r="C24" s="28">
+      <c r="D24" s="28">
         <v>4058.2968616666667</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="56">
         <v>44531</v>
       </c>
-      <c r="B25" s="28">
+      <c r="B25" s="32">
+        <v>0.84</v>
+      </c>
+      <c r="C25" s="28">
         <v>15029.246222222224</v>
       </c>
-      <c r="C25" s="28">
+      <c r="D25" s="28">
         <v>5861.4060266666675</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="56">
         <v>44562</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="32">
+        <v>0.83</v>
+      </c>
+      <c r="C26" s="28">
         <v>16695.665236111108</v>
       </c>
-      <c r="C26" s="28">
+      <c r="D26" s="28">
         <v>6511.3094420833331</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="56">
         <v>44593</v>
       </c>
-      <c r="B27" s="28">
+      <c r="B27" s="32">
+        <v>0.84</v>
+      </c>
+      <c r="C27" s="28">
         <v>10501.195586068377</v>
       </c>
-      <c r="C27" s="28">
+      <c r="D27" s="28">
         <v>4095.4662785666669</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="56">
         <v>44621</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="32">
+        <v>0.75</v>
+      </c>
+      <c r="C28" s="28">
         <v>12711.081841047679</v>
       </c>
-      <c r="C28" s="28">
+      <c r="D28" s="28">
         <v>4957.3219180085944</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="56">
         <v>44652</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="32">
+        <v>0.78</v>
+      </c>
+      <c r="C29" s="28">
         <v>16372.35923366013</v>
       </c>
-      <c r="C29" s="28">
+      <c r="D29" s="28">
         <v>6385.2201011274519</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="56">
         <v>44682</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="C30" s="28">
         <v>10097.578888888889</v>
       </c>
-      <c r="C30" s="28">
+      <c r="D30" s="28">
         <v>3938.0557666666664</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="56">
         <v>44713</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B31" s="32">
+        <v>0.54</v>
+      </c>
+      <c r="C31" s="28">
         <v>6489.1123076923068</v>
       </c>
-      <c r="C31" s="28">
+      <c r="D31" s="28">
         <v>2530.7537999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="56">
         <v>44743</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="32">
+        <v>0.83</v>
+      </c>
+      <c r="C32" s="28">
         <v>11764.787380952381</v>
       </c>
-      <c r="C32" s="28">
+      <c r="D32" s="28">
         <v>4588.267078571429</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="56">
         <v>44774</v>
       </c>
-      <c r="B33" s="28">
+      <c r="B33" s="32">
+        <v>0.62</v>
+      </c>
+      <c r="C33" s="28">
         <v>16500</v>
       </c>
-      <c r="C33" s="28">
+      <c r="D33" s="28">
         <v>6435</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="56">
         <v>44805</v>
       </c>
-      <c r="B34" s="28">
+      <c r="B34" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="C34" s="28">
         <v>9799.7923555555572</v>
       </c>
-      <c r="C34" s="28">
+      <c r="D34" s="28">
         <v>3821.9190186666674</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="56">
         <v>44835</v>
       </c>
-      <c r="B35" s="28">
+      <c r="B35" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="C35" s="28">
         <v>8493.9779262466673</v>
       </c>
-      <c r="C35" s="28">
+      <c r="D35" s="28">
         <v>3312.6513912362002</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="56">
         <v>44866</v>
       </c>
-      <c r="B36" s="28">
+      <c r="B36" s="32">
+        <v>0.65</v>
+      </c>
+      <c r="C36" s="28">
         <v>10405.889388888889</v>
       </c>
-      <c r="C36" s="28">
+      <c r="D36" s="28">
         <v>4058.2968616666667</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="56">
         <v>44896</v>
       </c>
-      <c r="B37" s="28">
+      <c r="B37" s="32">
+        <v>0.86</v>
+      </c>
+      <c r="C37" s="28">
         <v>14145.172915032683</v>
       </c>
-      <c r="C37" s="28">
+      <c r="D37" s="28">
         <v>5516.6174368627462</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="56">
         <v>44927</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="32">
+        <v>0.86</v>
+      </c>
+      <c r="C38" s="28">
         <v>17306.48225694444</v>
       </c>
-      <c r="C38" s="28">
+      <c r="D38" s="28">
         <v>6749.5280802083325</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="56">
         <v>44958</v>
       </c>
-      <c r="B39" s="28">
+      <c r="B39" s="32">
+        <v>0.87</v>
+      </c>
+      <c r="C39" s="28">
         <v>10971.398373504273</v>
       </c>
-      <c r="C39" s="28">
+      <c r="D39" s="28">
         <v>4278.8453656666661</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="56">
         <v>44986</v>
       </c>
-      <c r="B40" s="28">
+      <c r="B40" s="32">
+        <v>0.78</v>
+      </c>
+      <c r="C40" s="28">
         <v>13240.710251091332</v>
       </c>
-      <c r="C40" s="28">
+      <c r="D40" s="28">
         <v>5163.8769979256194</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="56">
         <v>45017</v>
       </c>
-      <c r="B41" s="28">
+      <c r="B41" s="32">
+        <v>0.78</v>
+      </c>
+      <c r="C41" s="28">
         <v>16971.347986111112</v>
       </c>
-      <c r="C41" s="28">
+      <c r="D41" s="28">
         <v>6618.825714583334</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="56">
         <v>45047</v>
       </c>
-      <c r="B42" s="28">
+      <c r="B42" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="C42" s="28">
         <v>12621.973611111112</v>
       </c>
-      <c r="C42" s="28">
+      <c r="D42" s="28">
         <v>4922.5697083333343</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="56">
         <v>45078</v>
       </c>
-      <c r="B43" s="28">
+      <c r="B43" s="32">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C43" s="28">
         <v>10544.807499999999</v>
       </c>
-      <c r="C43" s="28">
+      <c r="D43" s="28">
         <v>4112.4749249999995</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="56">
         <v>45108</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B44" s="32">
+        <v>0.83</v>
+      </c>
+      <c r="C44" s="28">
         <v>13725.585277777776</v>
       </c>
-      <c r="C44" s="28">
+      <c r="D44" s="28">
         <v>5352.9782583333326</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="56">
         <v>45139</v>
       </c>
-      <c r="B45" s="28">
+      <c r="B45" s="32">
+        <v>0.62</v>
+      </c>
+      <c r="C45" s="28">
         <v>11000</v>
       </c>
-      <c r="C45" s="28">
+      <c r="D45" s="28">
         <v>4290</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="56">
         <v>45170</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="C46" s="28">
         <v>9799.7923555555572</v>
       </c>
-      <c r="C46" s="28">
+      <c r="D46" s="28">
         <v>3821.9190186666674</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="56">
         <v>45200</v>
       </c>
-      <c r="B47" s="28">
-        <v>8493.9779262466673</v>
+      <c r="B47" s="32">
+        <v>0.4</v>
       </c>
       <c r="C47" s="28">
-        <v>3312.6513912362002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6500</v>
+      </c>
+      <c r="D47" s="28">
+        <f>C47*39%</f>
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="56">
         <v>45231</v>
       </c>
-      <c r="B48" s="28">
+      <c r="B48" s="32">
+        <v>0.68</v>
+      </c>
+      <c r="C48" s="28">
         <v>10405.889388888889</v>
       </c>
-      <c r="C48" s="28">
+      <c r="D48" s="28">
         <v>4058.2968616666667</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="56">
         <v>45261</v>
       </c>
-      <c r="B49" s="28">
+      <c r="B49" s="32">
+        <v>0.89</v>
+      </c>
+      <c r="C49" s="28">
         <v>15029.246222222224</v>
       </c>
-      <c r="C49" s="28">
+      <c r="D49" s="28">
         <v>5861.4060266666675</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="56">
         <v>45292</v>
       </c>
-      <c r="B50" s="28">
+      <c r="B50" s="32">
+        <v>0.86</v>
+      </c>
+      <c r="C50" s="28">
         <v>16695.665236111108</v>
       </c>
-      <c r="C50" s="28">
+      <c r="D50" s="28">
         <v>6511.3094420833331</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="56">
         <v>45323</v>
       </c>
-      <c r="B51" s="28">
+      <c r="B51" s="32">
+        <v>0.87</v>
+      </c>
+      <c r="C51" s="28">
         <v>10501.195586068377</v>
       </c>
-      <c r="C51" s="28">
+      <c r="D51" s="28">
         <v>4095.4662785666669</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="56">
         <v>45352</v>
       </c>
-      <c r="B52" s="28">
+      <c r="B52" s="32">
+        <v>0.78</v>
+      </c>
+      <c r="C52" s="28">
         <v>12711.081841047679</v>
       </c>
-      <c r="C52" s="28">
+      <c r="D52" s="28">
         <v>4957.3219180085944</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="56">
         <v>45383</v>
       </c>
-      <c r="B53" s="28">
+      <c r="B53" s="32">
+        <v>0.78</v>
+      </c>
+      <c r="C53" s="28">
         <v>16372.35923366013</v>
       </c>
-      <c r="C53" s="28">
+      <c r="D53" s="28">
         <v>6385.2201011274519</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="56">
         <v>45413</v>
       </c>
-      <c r="B54" s="28">
+      <c r="B54" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="C54" s="28">
         <v>10097.578888888889</v>
       </c>
-      <c r="C54" s="28">
+      <c r="D54" s="28">
         <v>3938.0557666666664</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="56">
         <v>45444</v>
       </c>
-      <c r="B55" s="28">
+      <c r="B55" s="32">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C55" s="28">
         <v>6489.1123076923068</v>
       </c>
-      <c r="C55" s="28">
+      <c r="D55" s="28">
         <v>2530.7537999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="56">
         <v>45474</v>
       </c>
-      <c r="B56" s="28">
+      <c r="B56" s="32">
+        <v>0.83</v>
+      </c>
+      <c r="C56" s="28">
         <v>11764.787380952381</v>
       </c>
-      <c r="C56" s="28">
+      <c r="D56" s="28">
         <v>4588.267078571429</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E56" s="63"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="56">
         <v>45505</v>
       </c>
-      <c r="B57" s="28">
+      <c r="B57" s="32">
+        <v>0.62</v>
+      </c>
+      <c r="C57" s="28">
         <v>16500</v>
       </c>
-      <c r="C57" s="28">
+      <c r="D57" s="28">
         <v>6435</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="56">
         <v>45536</v>
       </c>
-      <c r="B58" s="28">
+      <c r="B58" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="C58" s="28">
         <v>9799.7923555555572</v>
       </c>
-      <c r="C58" s="28">
+      <c r="D58" s="28">
         <v>3821.9190186666674</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="56">
         <v>45566</v>
       </c>
-      <c r="B59" s="28">
+      <c r="B59" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="C59" s="28">
         <v>8493.9779262466673</v>
       </c>
-      <c r="C59" s="28">
+      <c r="D59" s="28">
         <v>3312.6513912362002</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="56">
         <v>45597</v>
       </c>
-      <c r="B60" s="28">
+      <c r="B60" s="32">
+        <v>0.68</v>
+      </c>
+      <c r="C60" s="28">
         <v>10405.889388888889</v>
       </c>
-      <c r="C60" s="28">
+      <c r="D60" s="28">
         <v>4058.2968616666667</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="56">
         <v>45627</v>
       </c>
-      <c r="B61" s="28">
+      <c r="B61" s="32">
+        <v>0.89</v>
+      </c>
+      <c r="C61" s="28">
         <v>14145.172915032683</v>
       </c>
-      <c r="C61" s="28">
+      <c r="D61" s="28">
         <v>5516.6174368627462</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="56">
         <v>45658</v>
       </c>
-      <c r="B62" s="28">
+      <c r="B62" s="32">
+        <v>0.86</v>
+      </c>
+      <c r="C62" s="28">
         <v>17306.48225694444</v>
       </c>
-      <c r="C62" s="28">
+      <c r="D62" s="28">
         <v>6749.5280802083325</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="56">
         <v>45689</v>
       </c>
-      <c r="B63" s="28">
+      <c r="B63" s="32">
+        <v>0.87</v>
+      </c>
+      <c r="C63" s="28">
         <v>10971.398373504273</v>
       </c>
-      <c r="C63" s="28">
+      <c r="D63" s="28">
         <v>4278.8453656666661</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="56">
         <v>45717</v>
       </c>
-      <c r="B64" s="28">
+      <c r="B64" s="32">
+        <v>0.78</v>
+      </c>
+      <c r="C64" s="28">
         <v>13240.710251091332</v>
       </c>
-      <c r="C64" s="28">
+      <c r="D64" s="28">
         <v>5163.8769979256194</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="56">
         <v>45748</v>
       </c>
-      <c r="B65" s="28">
+      <c r="B65" s="32">
+        <v>0.78</v>
+      </c>
+      <c r="C65" s="28">
         <v>16971.347986111112</v>
       </c>
-      <c r="C65" s="28">
+      <c r="D65" s="28">
         <v>6618.825714583334</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="56">
         <v>45778</v>
       </c>
-      <c r="B66" s="28">
+      <c r="B66" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="C66" s="28">
         <v>12621.973611111112</v>
       </c>
-      <c r="C66" s="28">
+      <c r="D66" s="28">
         <v>4922.5697083333343</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="56">
         <v>45809</v>
       </c>
-      <c r="B67" s="28">
-        <v>10544.807499999999</v>
+      <c r="B67" s="32">
+        <v>0.56999999999999995</v>
       </c>
       <c r="C67" s="28">
+        <v>8000</v>
+      </c>
+      <c r="D67" s="28">
         <v>4112.4749249999995</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="56">
         <v>45839</v>
       </c>
-      <c r="B68" s="28">
+      <c r="B68" s="32">
+        <v>0.83</v>
+      </c>
+      <c r="C68" s="28">
         <v>13725.585277777776</v>
       </c>
-      <c r="C68" s="28">
+      <c r="D68" s="28">
         <v>5352.9782583333326</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E68" s="63"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="56">
         <v>45870</v>
       </c>
-      <c r="B69" s="28">
+      <c r="B69" s="32">
+        <v>0.62</v>
+      </c>
+      <c r="C69" s="28">
         <v>11000</v>
       </c>
-      <c r="C69" s="28">
+      <c r="D69" s="28">
         <v>4290</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="56">
         <v>45901</v>
       </c>
-      <c r="B70" s="28">
+      <c r="B70" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="C70" s="28">
         <v>9799.7923555555572</v>
       </c>
-      <c r="C70" s="28">
+      <c r="D70" s="28">
         <v>3821.9190186666674</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="56">
         <v>45931</v>
       </c>
-      <c r="B71" s="28">
-        <v>8493.9779262466673</v>
+      <c r="B71" s="32">
+        <v>0.4</v>
       </c>
       <c r="C71" s="28">
-        <v>3312.6513912362002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7000</v>
+      </c>
+      <c r="D71" s="28">
+        <f>C71*39%</f>
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="56">
         <v>45962</v>
       </c>
-      <c r="B72" s="28">
+      <c r="B72" s="32">
+        <v>0.68</v>
+      </c>
+      <c r="C72" s="28">
         <v>10405.889388888889</v>
       </c>
-      <c r="C72" s="28">
+      <c r="D72" s="28">
         <v>4058.2968616666667</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="56">
         <v>45992</v>
       </c>
-      <c r="B73" s="28">
+      <c r="B73" s="32">
+        <v>0.89</v>
+      </c>
+      <c r="C73" s="28">
         <v>15029.246222222224</v>
       </c>
-      <c r="C73" s="28">
+      <c r="D73" s="28">
         <v>5861.4060266666675</v>
       </c>
     </row>
@@ -16994,555 +17258,703 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8FDAEC-D40F-7442-9EF7-1FD49F660D8C}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="55"/>
-    <col min="2" max="2" width="23" style="55" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="55"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="55" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="56">
+      <c r="D1" s="28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="64">
         <v>44562</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="67">
+        <v>0.61</v>
+      </c>
+      <c r="C2" s="65">
         <v>13136.888888888889</v>
       </c>
-      <c r="C2" s="28">
+      <c r="D2" s="65">
         <v>1471</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="56">
+    <row r="3" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="64">
         <v>44593</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="67">
+        <v>0.62</v>
+      </c>
+      <c r="C3" s="65">
         <v>11430.527777777777</v>
       </c>
-      <c r="C3" s="28">
+      <c r="D3" s="65">
         <v>935.38888888888891</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="56">
+    <row r="4" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="64">
         <v>44621</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="67">
+        <v>0.39</v>
+      </c>
+      <c r="C4" s="65">
         <v>9742.6111111111113</v>
       </c>
-      <c r="C4" s="28">
+      <c r="D4" s="65">
         <v>1150.5555555555557</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="56">
+    <row r="5" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="64">
         <v>44652</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="67">
+        <v>0.7</v>
+      </c>
+      <c r="C5" s="65">
         <v>15043.805555555555</v>
       </c>
-      <c r="C5" s="28">
+      <c r="D5" s="65">
         <v>2108</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="56">
+    <row r="6" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="64">
         <v>44682</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="67">
+        <v>0.47</v>
+      </c>
+      <c r="C6" s="65">
         <v>8546.1691666666666</v>
       </c>
-      <c r="C6" s="28">
+      <c r="D6" s="65">
         <v>861.11111111111109</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="56">
+    <row r="7" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="64">
         <v>44713</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="67">
+        <v>0.33</v>
+      </c>
+      <c r="C7" s="65">
         <v>7171.4191666666666</v>
       </c>
-      <c r="C7" s="28">
+      <c r="D7" s="65">
         <v>972.22222222222217</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="56">
+    <row r="8" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="64">
         <v>44743</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="67">
+        <v>0.67</v>
+      </c>
+      <c r="C8" s="65">
         <v>15864.97388888889</v>
       </c>
-      <c r="C8" s="28">
+      <c r="D8" s="65">
         <v>2219.1705555555554</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="56">
+    <row r="9" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="64">
         <v>44774</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="67">
+        <v>0.49</v>
+      </c>
+      <c r="C9" s="65">
         <v>11925.820833333333</v>
       </c>
-      <c r="C9" s="28">
+      <c r="D9" s="65">
         <v>1249.3127776333333</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="56">
+    <row r="10" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="64">
         <v>44805</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="67">
+        <v>0.51</v>
+      </c>
+      <c r="C10" s="65">
         <v>13738.026666666667</v>
       </c>
-      <c r="C10" s="28">
+      <c r="D10" s="65">
         <v>431.60242055555557</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="56">
+    <row r="11" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="64">
         <v>44835</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="67">
+        <v>0.4</v>
+      </c>
+      <c r="C11" s="65">
         <v>7765.7254499999999</v>
       </c>
-      <c r="C11" s="28">
+      <c r="D11" s="65">
         <v>619.92006944444449</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="56">
+    <row r="12" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="64">
         <v>44866</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="67">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C12" s="65">
         <v>14796.252777777778</v>
       </c>
-      <c r="C12" s="28">
+      <c r="D12" s="65">
         <v>787.54525466666666</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="56">
+    <row r="13" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="64">
         <v>44896</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="67">
+        <v>0.79</v>
+      </c>
+      <c r="C13" s="65">
         <v>16039.116388888888</v>
       </c>
-      <c r="C13" s="28">
+      <c r="D13" s="65">
         <v>525.37747777777497</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="56">
+    <row r="14" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="64">
         <v>44927</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="67">
+        <v>0.81</v>
+      </c>
+      <c r="C14" s="65">
         <v>18609.989444444444</v>
       </c>
-      <c r="C14" s="28">
+      <c r="D14" s="65">
         <v>2203.6549999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="56">
+    <row r="15" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="64">
         <v>44958</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="67">
+        <v>0.82</v>
+      </c>
+      <c r="C15" s="65">
         <v>16622.081111111111</v>
       </c>
-      <c r="C15" s="28">
+      <c r="D15" s="65">
         <v>1691.2816666666668</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="56">
+    <row r="16" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="64">
         <v>44986</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="67">
+        <v>0.78</v>
+      </c>
+      <c r="C16" s="65">
         <v>21306.423360019777</v>
       </c>
-      <c r="C16" s="28">
+      <c r="D16" s="65">
         <v>1902.1211111111106</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="56">
+    <row r="17" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="64">
         <v>45017</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="67">
+        <v>0.73</v>
+      </c>
+      <c r="C17" s="65">
         <v>17039.369466666667</v>
       </c>
-      <c r="C17" s="28">
+      <c r="D17" s="65">
         <v>2049.2951111111111</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="56">
+    <row r="18" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="64">
         <v>45047</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="67">
+        <v>0.6</v>
+      </c>
+      <c r="C18" s="65">
         <v>16731.527777777777</v>
       </c>
-      <c r="C18" s="28">
+      <c r="D18" s="65">
         <v>1519.95955</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="56">
+    <row r="19" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="64">
         <v>45078</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="67">
+        <v>0.52</v>
+      </c>
+      <c r="C19" s="65">
         <v>15332.020833333334</v>
       </c>
-      <c r="C19" s="28">
+      <c r="D19" s="65">
         <v>1344.8148138888889</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="56">
+    <row r="20" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="64">
         <v>45108</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="67">
+        <v>0.83</v>
+      </c>
+      <c r="C20" s="65">
         <v>20746.446944444444</v>
       </c>
-      <c r="C20" s="28">
+      <c r="D20" s="65">
         <v>1833.3412722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="56">
+    <row r="21" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="64">
         <v>45139</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="67">
+        <v>0.62</v>
+      </c>
+      <c r="C21" s="65">
         <v>17000</v>
       </c>
-      <c r="C21" s="28">
+      <c r="D21" s="65">
         <v>1700</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="56">
+    <row r="22" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="64">
         <v>45170</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="68">
+        <v>0.7</v>
+      </c>
+      <c r="C22" s="65">
         <v>14699.688533333334</v>
       </c>
-      <c r="C22" s="28">
+      <c r="D22" s="65">
         <v>1469.9688533333335</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="56">
+    <row r="23" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="64">
         <v>45200</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="68">
+        <v>0.4</v>
+      </c>
+      <c r="C23" s="65">
         <v>8309.3262315000011</v>
       </c>
-      <c r="C23" s="28">
+      <c r="D23" s="65">
         <v>830.93262315000015</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="56">
+    <row r="24" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="64">
         <v>45231</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="68">
+        <v>0.63</v>
+      </c>
+      <c r="C24" s="65">
         <v>16275.878055555557</v>
       </c>
-      <c r="C24" s="28">
+      <c r="D24" s="65">
         <v>1627.5878055555559</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="56">
+    <row r="25" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="64">
         <v>45261</v>
       </c>
-      <c r="B25" s="28">
+      <c r="B25" s="68">
+        <v>0.84</v>
+      </c>
+      <c r="C25" s="65">
         <v>17643.028027777778</v>
       </c>
-      <c r="C25" s="28">
+      <c r="D25" s="65">
         <v>1764.302802777778</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="56">
+    <row r="26" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="64">
         <v>45292</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="67">
+        <v>0.83</v>
+      </c>
+      <c r="C26" s="65">
         <v>19069.495356652948</v>
       </c>
-      <c r="C26" s="28">
+      <c r="D26" s="65">
         <v>1906.9495356652949</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="56">
+    <row r="27" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="64">
         <v>45323</v>
       </c>
-      <c r="B27" s="28">
+      <c r="B27" s="67">
+        <v>0.84</v>
+      </c>
+      <c r="C27" s="65">
         <v>17027.497723577235</v>
       </c>
-      <c r="C27" s="28">
+      <c r="D27" s="65">
         <v>1702.7497723577235</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="56">
+    <row r="28" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" s="64">
         <v>45352</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="67">
+        <v>0.75</v>
+      </c>
+      <c r="C28" s="65">
         <v>20486.945538480555</v>
       </c>
-      <c r="C28" s="28">
+      <c r="D28" s="65">
         <v>2048.6945538480554</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="56">
+    <row r="29" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="64">
         <v>45383</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="67">
+        <v>0.78</v>
+      </c>
+      <c r="C29" s="65">
         <v>17039.369466666667</v>
       </c>
-      <c r="C29" s="28">
+      <c r="D29" s="65">
         <v>1703.9369466666667</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="56">
+    <row r="30" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="64">
         <v>45413</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="67">
+        <v>0.6</v>
+      </c>
+      <c r="C30" s="65">
         <v>16731.527777777777</v>
       </c>
-      <c r="C30" s="28">
+      <c r="D30" s="65">
         <v>1673.1527777777778</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="56">
+    <row r="31" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="64">
         <v>45444</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B31" s="67">
+        <v>0.54</v>
+      </c>
+      <c r="C31" s="65">
         <v>15332.020833333334</v>
       </c>
-      <c r="C31" s="28">
+      <c r="D31" s="65">
         <v>1533.2020833333336</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="56">
+    <row r="32" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" s="64">
         <v>45474</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="67">
+        <v>0.83</v>
+      </c>
+      <c r="C32" s="65">
         <v>20746.446944444444</v>
       </c>
-      <c r="C32" s="28">
+      <c r="D32" s="65">
         <v>2074.6446944444447</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="56">
+    <row r="33" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="64">
         <v>45505</v>
       </c>
-      <c r="B33" s="28">
+      <c r="B33" s="67">
+        <v>0.62</v>
+      </c>
+      <c r="C33" s="65">
         <v>17000</v>
       </c>
-      <c r="C33" s="28">
+      <c r="D33" s="65">
         <v>1700</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="56">
+    <row r="34" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="64">
         <v>45536</v>
       </c>
-      <c r="B34" s="28">
+      <c r="B34" s="68">
+        <v>0.7</v>
+      </c>
+      <c r="C34" s="65">
         <v>15728.666730666668</v>
       </c>
-      <c r="C34" s="28">
+      <c r="D34" s="65">
         <v>1572.8666730666669</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="56">
+    <row r="35" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="64">
         <v>45566</v>
       </c>
-      <c r="B35" s="28">
+      <c r="B35" s="68">
+        <v>0.4</v>
+      </c>
+      <c r="C35" s="65">
         <v>8890.9790677050023</v>
       </c>
-      <c r="C35" s="28">
+      <c r="D35" s="65">
         <v>889.09790677050023</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="56">
+    <row r="36" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="64">
         <v>45597</v>
       </c>
-      <c r="B36" s="28">
+      <c r="B36" s="68">
+        <v>0.65</v>
+      </c>
+      <c r="C36" s="65">
         <v>16792.572597001767</v>
       </c>
-      <c r="C36" s="28">
+      <c r="D36" s="65">
         <v>1679.2572597001767</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="56">
+    <row r="37" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="64">
         <v>45627</v>
       </c>
-      <c r="B37" s="28">
+      <c r="B37" s="68">
+        <v>0.86</v>
+      </c>
+      <c r="C37" s="65">
         <v>18063.10012367725</v>
       </c>
-      <c r="C37" s="28">
+      <c r="D37" s="65">
         <v>1806.310012367725</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="56">
+    <row r="38" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="64">
         <v>45658</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="67">
+        <v>0.86</v>
+      </c>
+      <c r="C38" s="65">
         <v>19758.754224965702</v>
       </c>
-      <c r="C38" s="28">
+      <c r="D38" s="65">
         <v>1975.8754224965703</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="56">
+    <row r="39" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="64">
         <v>45689</v>
       </c>
-      <c r="B39" s="28">
+      <c r="B39" s="67">
+        <v>0.87</v>
+      </c>
+      <c r="C39" s="65">
         <v>17635.622642276423</v>
       </c>
-      <c r="C39" s="28">
+      <c r="D39" s="65">
         <v>1763.5622642276423</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="56">
+    <row r="40" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="64">
         <v>45717</v>
       </c>
-      <c r="B40" s="28">
+      <c r="B40" s="67">
+        <v>0.78</v>
+      </c>
+      <c r="C40" s="65">
         <v>21306.42336001978</v>
       </c>
-      <c r="C40" s="28">
+      <c r="D40" s="65">
         <v>2130.642336001978</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="56">
+    <row r="41" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="64">
         <v>45748</v>
       </c>
-      <c r="B41" s="28">
+      <c r="B41" s="67">
+        <v>0.78</v>
+      </c>
+      <c r="C41" s="65">
         <v>17039.369466666667</v>
       </c>
-      <c r="C41" s="28">
+      <c r="D41" s="65">
         <v>1703.9369466666667</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="56">
+    <row r="42" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="64">
         <v>45778</v>
       </c>
-      <c r="B42" s="28">
+      <c r="B42" s="67">
+        <v>0.6</v>
+      </c>
+      <c r="C42" s="65">
         <v>15221.290384516129</v>
       </c>
-      <c r="C42" s="28">
+      <c r="D42" s="65">
         <v>1522.129038451613</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="56">
+    <row r="43" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="64">
         <v>45809</v>
       </c>
-      <c r="B43" s="28">
+      <c r="B43" s="67">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C43" s="65">
         <v>14460.225865290322</v>
       </c>
-      <c r="C43" s="28">
+      <c r="D43" s="65">
         <v>1446.0225865290322</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="56">
+    <row r="44" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="64">
         <v>45839</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B44" s="67">
+        <v>0.83</v>
+      </c>
+      <c r="C44" s="65">
         <v>20746.446944444444</v>
       </c>
-      <c r="C44" s="28">
+      <c r="D44" s="65">
         <v>2074.6446944444447</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="56">
+    <row r="45" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="64">
         <v>45870</v>
       </c>
-      <c r="B45" s="28">
+      <c r="B45" s="67">
+        <v>0.62</v>
+      </c>
+      <c r="C45" s="65">
         <v>17000</v>
       </c>
-      <c r="C45" s="28">
+      <c r="D45" s="65">
         <v>1700</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="56">
+    <row r="46" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="64">
         <v>45901</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="C46" s="65">
         <v>15728.666730666668</v>
       </c>
-      <c r="C46" s="28">
+      <c r="D46" s="65">
         <v>1572.8666730666669</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="56">
+    <row r="47" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A47" s="64">
         <v>45931</v>
       </c>
-      <c r="B47" s="28">
+      <c r="B47" s="69">
+        <v>0.4</v>
+      </c>
+      <c r="C47" s="65">
         <v>8890.9790677050023</v>
       </c>
-      <c r="C47" s="28">
+      <c r="D47" s="65">
         <v>889.09790677050023</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="56">
+    <row r="48" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A48" s="64">
         <v>45962</v>
       </c>
-      <c r="B48" s="28">
+      <c r="B48" s="69">
+        <v>0.68</v>
+      </c>
+      <c r="C48" s="65">
         <v>15114.664415098505</v>
       </c>
-      <c r="C48" s="28">
+      <c r="D48" s="65">
         <v>1511.4664415098505</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="56">
+    <row r="49" spans="1:4" s="66" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="64">
         <v>45992</v>
       </c>
-      <c r="B49" s="28">
+      <c r="B49" s="69">
+        <v>0.89</v>
+      </c>
+      <c r="C49" s="65">
         <v>18693.208267526457</v>
       </c>
-      <c r="C49" s="28">
+      <c r="D49" s="65">
         <v>1869.3208267526459</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bugs in the app
</commit_message>
<xml_diff>
--- a/budgetusd.xlsx
+++ b/budgetusd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielporras/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED76ABC0-06F3-F242-8A12-56941A439290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7DEB32-F9C4-DD4E-A805-970277900EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="600" windowWidth="25020" windowHeight="15840" activeTab="3" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{26BE6A92-8F4C-F74C-A2D9-BBF367B42B22}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -4715,7 +4715,7 @@
         <v>9</v>
       </c>
       <c r="K26" s="16">
-        <f>(((B26*K14)/B14)*(1+(I26-I14)/I14))</f>
+        <f t="shared" ref="K26:K36" si="0">(((B26*K14)/B14)*(1+(I26-I14)/I14))</f>
         <v>8471.7004909090901</v>
       </c>
     </row>
@@ -4751,7 +4751,7 @@
         <v>9</v>
       </c>
       <c r="K27" s="16">
-        <f>(((B27*K15)/B15)*(1+(I27-I15)/I15))</f>
+        <f t="shared" si="0"/>
         <v>16948.435000000001</v>
       </c>
     </row>
@@ -4787,7 +4787,7 @@
         <v>9</v>
       </c>
       <c r="K28" s="16">
-        <f>(((B28*K16)/B16)*(1+(I28-I16)/I16))</f>
+        <f t="shared" si="0"/>
         <v>18604.636731875715</v>
       </c>
     </row>
@@ -4823,7 +4823,7 @@
         <v>9</v>
       </c>
       <c r="K29" s="16">
-        <f>(((B29*K17)/B17)*(1+(I29-I17)/I17))</f>
+        <f t="shared" si="0"/>
         <v>20261.338816443757</v>
       </c>
     </row>
@@ -4859,7 +4859,7 @@
         <v>9</v>
       </c>
       <c r="K30" s="16">
-        <f>(((B30*K18)/B18)*(1+(I30-I18)/I18))</f>
+        <f t="shared" si="0"/>
         <v>18091.716331300813</v>
       </c>
     </row>
@@ -4895,7 +4895,7 @@
         <v>9</v>
       </c>
       <c r="K31" s="16">
-        <f>(((B31*K19)/B19)*(1+(I31-I19)/I19))</f>
+        <f t="shared" si="0"/>
         <v>20980.606876757196</v>
       </c>
     </row>
@@ -4931,7 +4931,7 @@
         <v>9</v>
       </c>
       <c r="K32" s="16">
-        <f>(((B32*K20)/B20)*(1+(I32-I20)/I20))</f>
+        <f t="shared" si="0"/>
         <v>19344.352665068498</v>
       </c>
     </row>
@@ -4967,7 +4967,7 @@
         <v>9</v>
       </c>
       <c r="K33" s="16">
-        <f>(((B33*K21)/B21)*(1+(I33-I21)/I21))</f>
+        <f t="shared" si="0"/>
         <v>17777.248263888887</v>
       </c>
     </row>
@@ -5003,7 +5003,7 @@
         <v>9</v>
       </c>
       <c r="K34" s="16">
-        <f>(((B34*K22)/B22)*(1+(I34-I22)/I22))</f>
+        <f t="shared" si="0"/>
         <v>16916.821063701922</v>
       </c>
     </row>
@@ -5039,7 +5039,7 @@
         <v>9</v>
       </c>
       <c r="K35" s="16">
-        <f>(((B35*K23)/B23)*(1+(I35-I23)/I23))</f>
+        <f t="shared" si="0"/>
         <v>22043.099878472221</v>
       </c>
     </row>
@@ -5075,7 +5075,7 @@
         <v>9</v>
       </c>
       <c r="K36" s="16">
-        <f>(((B36*K24)/B24)*(1+(I36-I24)/I24))</f>
+        <f t="shared" si="0"/>
         <v>17202.38095238095</v>
       </c>
     </row>
@@ -5111,7 +5111,7 @@
         <v>9</v>
       </c>
       <c r="K37" s="16">
-        <f t="shared" ref="K37:K52" si="0">(((B37*K25)/B25)*(1+(I37-I25)/I25))</f>
+        <f t="shared" ref="K37:K52" si="1">(((B37*K25)/B25)*(1+(I37-I25)/I25))</f>
         <v>19080.684583934581</v>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
         <v>9</v>
       </c>
       <c r="K38" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9644.1233267045445</v>
       </c>
     </row>
@@ -5183,7 +5183,7 @@
         <v>9</v>
       </c>
       <c r="K39" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17902.825330687832</v>
       </c>
     </row>
@@ -5219,7 +5219,7 @@
         <v>9</v>
       </c>
       <c r="K40" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19501.11866056587</v>
       </c>
     </row>
@@ -5255,7 +5255,7 @@
         <v>9</v>
       </c>
       <c r="K41" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21240.660791838131</v>
       </c>
     </row>
@@ -5291,7 +5291,7 @@
         <v>9</v>
       </c>
       <c r="K42" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18958.294340447155</v>
       </c>
     </row>
@@ -5327,7 +5327,7 @@
         <v>9</v>
       </c>
       <c r="K43" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22076.535047731333</v>
       </c>
     </row>
@@ -5363,7 +5363,7 @@
         <v>9</v>
       </c>
       <c r="K44" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19571.933284657538</v>
       </c>
     </row>
@@ -5399,7 +5399,7 @@
         <v>9</v>
       </c>
       <c r="K45" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17986.392361111109</v>
       </c>
     </row>
@@ -5435,7 +5435,7 @@
         <v>9</v>
       </c>
       <c r="K46" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18066.722626201918</v>
       </c>
     </row>
@@ -5471,7 +5471,7 @@
         <v>9</v>
       </c>
       <c r="K47" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22302.430465277776</v>
       </c>
     </row>
@@ -5507,7 +5507,7 @@
         <v>9</v>
       </c>
       <c r="K48" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17404.761904761901</v>
       </c>
     </row>
@@ -5543,7 +5543,7 @@
         <v>9</v>
       </c>
       <c r="K49" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19305.163226098517</v>
       </c>
     </row>
@@ -5579,7 +5579,7 @@
         <v>9</v>
       </c>
       <c r="K50" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8673.4076454545429</v>
       </c>
     </row>
@@ -5615,7 +5615,7 @@
         <v>9</v>
       </c>
       <c r="K51" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18946.889920634923</v>
       </c>
     </row>
@@ -5651,7 +5651,7 @@
         <v>9</v>
       </c>
       <c r="K52" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20416.057570140823</v>
       </c>
     </row>
@@ -5665,8 +5665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3125D8-EE63-4B43-9AC6-51D16219A8B2}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="139" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="139" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6566,10 +6566,10 @@
         <v>59</v>
       </c>
       <c r="B24" s="28">
-        <v>0.62</v>
+        <v>0.59</v>
       </c>
       <c r="C24" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>50</v>
@@ -6581,13 +6581,13 @@
         <v>46</v>
       </c>
       <c r="G24" s="24">
-        <v>319.48371291666666</v>
+        <v>300</v>
       </c>
       <c r="H24" s="24">
         <v>9</v>
       </c>
       <c r="I24" s="24">
-        <v>17000</v>
+        <v>16965</v>
       </c>
       <c r="J24" s="33">
         <v>0.4</v>
@@ -6596,7 +6596,7 @@
         <v>20</v>
       </c>
       <c r="L24" s="18">
-        <v>11000</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.25">
@@ -7060,7 +7060,7 @@
       </c>
       <c r="L36" s="19">
         <f t="shared" si="1"/>
-        <v>16500</v>
+        <v>18750</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="21" x14ac:dyDescent="0.25">
@@ -7528,7 +7528,7 @@
       </c>
       <c r="L48" s="19">
         <f t="shared" si="1"/>
-        <v>11000</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="21" x14ac:dyDescent="0.25">

</xml_diff>